<commit_message>
mise à jour outil conversion
</commit_message>
<xml_diff>
--- a/migration_bdd.xlsx
+++ b/migration_bdd.xlsx
@@ -16,10 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="306">
-  <si>
-    <t>Tableau des correspondances entre l2jfree 5839 et l2j 4422</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="306">
   <si>
     <t>X</t>
   </si>
@@ -921,19 +918,22 @@
     <t>messages</t>
   </si>
   <si>
-    <t>oui</t>
-  </si>
-  <si>
-    <t>non</t>
-  </si>
-  <si>
-    <t>SQL</t>
-  </si>
-  <si>
-    <t>Différences</t>
-  </si>
-  <si>
     <t>ALTER TABLE clan_data MODIFY COLUMN reputation_score int(11) AFTER clan_level</t>
+  </si>
+  <si>
+    <t>utiliser les données de item_attributes</t>
+  </si>
+  <si>
+    <t>Numéro</t>
+  </si>
+  <si>
+    <t>Tableau des correspondances entre l2jfree 5839 et l2j 4422 ; tables critiques en gris, à chaque requête SQL correspond un numéro</t>
+  </si>
+  <si>
+    <t>identique</t>
+  </si>
+  <si>
+    <t>SQL de CONVERSION</t>
   </si>
 </sst>
 </file>
@@ -1221,7 +1221,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1254,13 +1254,28 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1269,28 +1284,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -1309,6 +1306,10 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1606,8 +1607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B3:E186"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B43" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E66" sqref="E66"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1619,1955 +1620,1990 @@
   <sheetData>
     <row r="3" spans="2:5" ht="16.5" thickBot="1">
       <c r="B3" s="3" t="s">
-        <v>0</v>
+        <v>303</v>
       </c>
     </row>
     <row r="4" spans="2:5" ht="16.5" thickBot="1">
       <c r="B4" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>298</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>299</v>
-      </c>
       <c r="D4" s="7" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
     </row>
     <row r="5" spans="2:5">
       <c r="B5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="25"/>
-      <c r="E5" s="26"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="15"/>
     </row>
     <row r="6" spans="2:5">
       <c r="B6" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>301</v>
+      <c r="D6" s="9">
+        <v>1</v>
       </c>
       <c r="E6" s="10"/>
     </row>
     <row r="7" spans="2:5">
       <c r="B7" s="8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="15" t="s">
-        <v>302</v>
-      </c>
-      <c r="E7" s="16"/>
+        <v>4</v>
+      </c>
+      <c r="D7" s="24" t="s">
+        <v>304</v>
+      </c>
+      <c r="E7" s="25"/>
     </row>
     <row r="8" spans="2:5">
       <c r="B8" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="19"/>
-      <c r="E8" s="20"/>
+        <v>5</v>
+      </c>
+      <c r="D8" s="16"/>
+      <c r="E8" s="17"/>
     </row>
     <row r="9" spans="2:5">
       <c r="B9" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="23"/>
-      <c r="E9" s="24"/>
+        <v>6</v>
+      </c>
+      <c r="D9" s="18"/>
+      <c r="E9" s="19"/>
     </row>
     <row r="10" spans="2:5">
       <c r="B10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="23"/>
-      <c r="E10" s="24"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="19"/>
     </row>
     <row r="11" spans="2:5">
       <c r="B11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="23"/>
-      <c r="E11" s="24"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="19"/>
     </row>
     <row r="12" spans="2:5">
       <c r="B12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" s="23"/>
-      <c r="E12" s="24"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="19"/>
     </row>
     <row r="13" spans="2:5">
       <c r="B13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" s="23"/>
-      <c r="E13" s="24"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="19"/>
     </row>
     <row r="14" spans="2:5">
       <c r="B14" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D14" s="23"/>
-      <c r="E14" s="24"/>
+        <v>0</v>
+      </c>
+      <c r="D14" s="18"/>
+      <c r="E14" s="19"/>
     </row>
     <row r="15" spans="2:5">
       <c r="B15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15" s="23"/>
-      <c r="E15" s="24"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="19"/>
     </row>
     <row r="16" spans="2:5">
       <c r="B16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D16" s="23"/>
-      <c r="E16" s="24"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="19"/>
     </row>
     <row r="17" spans="2:5">
       <c r="B17" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D17" s="23"/>
-      <c r="E17" s="24"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="19"/>
     </row>
     <row r="18" spans="2:5">
       <c r="B18" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D18" s="23"/>
-      <c r="E18" s="24"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="19"/>
     </row>
     <row r="19" spans="2:5">
       <c r="B19" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D19" s="21"/>
-      <c r="E19" s="22"/>
+        <v>0</v>
+      </c>
+      <c r="D19" s="20"/>
+      <c r="E19" s="21"/>
     </row>
     <row r="20" spans="2:5">
       <c r="B20" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>301</v>
+      <c r="D20" s="9">
+        <v>2</v>
       </c>
       <c r="E20" s="10"/>
     </row>
     <row r="21" spans="2:5">
       <c r="B21" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D21" s="19"/>
-      <c r="E21" s="20"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="17"/>
     </row>
     <row r="22" spans="2:5">
       <c r="B22" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D22" s="21"/>
-      <c r="E22" s="22"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="21"/>
     </row>
     <row r="23" spans="2:5">
       <c r="B23" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C23" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>301</v>
+      <c r="D23" s="9">
+        <v>3</v>
       </c>
       <c r="E23" s="10"/>
     </row>
     <row r="24" spans="2:5">
       <c r="B24" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D24" s="17"/>
-      <c r="E24" s="18"/>
+        <v>0</v>
+      </c>
+      <c r="D24" s="22"/>
+      <c r="E24" s="23"/>
     </row>
     <row r="25" spans="2:5">
       <c r="B25" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C25" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>301</v>
+      <c r="D25" s="9">
+        <v>4</v>
       </c>
       <c r="E25" s="10"/>
     </row>
     <row r="26" spans="2:5">
       <c r="B26" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C26" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C26" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>301</v>
+      <c r="D26" s="9">
+        <v>5</v>
       </c>
       <c r="E26" s="10"/>
     </row>
     <row r="27" spans="2:5">
       <c r="B27" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D27" s="19"/>
-      <c r="E27" s="20"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="17"/>
     </row>
     <row r="28" spans="2:5">
       <c r="B28" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D28" s="23"/>
-      <c r="E28" s="24"/>
+        <v>0</v>
+      </c>
+      <c r="D28" s="18"/>
+      <c r="E28" s="19"/>
     </row>
     <row r="29" spans="2:5">
       <c r="B29" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D29" s="23"/>
-      <c r="E29" s="24"/>
+        <v>0</v>
+      </c>
+      <c r="D29" s="18"/>
+      <c r="E29" s="19"/>
     </row>
     <row r="30" spans="2:5">
       <c r="B30" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D30" s="21"/>
-      <c r="E30" s="22"/>
+        <v>0</v>
+      </c>
+      <c r="D30" s="20"/>
+      <c r="E30" s="21"/>
     </row>
     <row r="31" spans="2:5">
       <c r="B31" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C31" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C31" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="D31" s="9" t="s">
-        <v>301</v>
+      <c r="D31" s="9">
+        <v>6</v>
       </c>
       <c r="E31" s="10"/>
     </row>
     <row r="32" spans="2:5">
       <c r="B32" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="D32" s="15" t="s">
-        <v>302</v>
-      </c>
-      <c r="E32" s="16"/>
+        <v>0</v>
+      </c>
+      <c r="D32" s="24" t="s">
+        <v>304</v>
+      </c>
+      <c r="E32" s="25"/>
     </row>
     <row r="33" spans="2:5">
       <c r="B33" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="D33" s="15" t="s">
-        <v>302</v>
-      </c>
-      <c r="E33" s="16"/>
+        <v>0</v>
+      </c>
+      <c r="D33" s="24" t="s">
+        <v>304</v>
+      </c>
+      <c r="E33" s="25"/>
     </row>
     <row r="34" spans="2:5">
       <c r="B34" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="D34" s="15" t="s">
-        <v>302</v>
-      </c>
-      <c r="E34" s="16"/>
+        <v>0</v>
+      </c>
+      <c r="D34" s="24" t="s">
+        <v>304</v>
+      </c>
+      <c r="E34" s="25"/>
     </row>
     <row r="35" spans="2:5">
       <c r="B35" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C35" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="C35" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="D35" s="9" t="s">
-        <v>301</v>
+      <c r="D35" s="9">
+        <v>7</v>
       </c>
       <c r="E35" s="10"/>
     </row>
     <row r="36" spans="2:5">
       <c r="B36" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C36" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="C36" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="D36" s="9" t="s">
-        <v>301</v>
+      <c r="D36" s="9">
+        <v>8</v>
       </c>
       <c r="E36" s="10"/>
     </row>
     <row r="37" spans="2:5">
       <c r="B37" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C37" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C37" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="D37" s="9" t="s">
-        <v>301</v>
+      <c r="D37" s="9">
+        <v>9</v>
       </c>
       <c r="E37" s="10"/>
     </row>
     <row r="38" spans="2:5">
       <c r="B38" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C38" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="C38" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="D38" s="15" t="s">
-        <v>302</v>
-      </c>
-      <c r="E38" s="16"/>
+      <c r="D38" s="24" t="s">
+        <v>304</v>
+      </c>
+      <c r="E38" s="25"/>
     </row>
     <row r="39" spans="2:5">
       <c r="B39" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>300</v>
-      </c>
-      <c r="D39" s="9" t="s">
-        <v>301</v>
+        <v>299</v>
+      </c>
+      <c r="D39" s="9">
+        <v>10</v>
       </c>
       <c r="E39" s="10"/>
     </row>
     <row r="40" spans="2:5">
       <c r="B40" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="D40" s="15" t="s">
-        <v>302</v>
-      </c>
-      <c r="E40" s="16"/>
+        <v>0</v>
+      </c>
+      <c r="D40" s="24" t="s">
+        <v>304</v>
+      </c>
+      <c r="E40" s="25"/>
     </row>
     <row r="41" spans="2:5">
       <c r="B41" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D41" s="17"/>
-      <c r="E41" s="18"/>
+        <v>58</v>
+      </c>
+      <c r="D41" s="22"/>
+      <c r="E41" s="23"/>
     </row>
     <row r="42" spans="2:5">
       <c r="B42" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C42" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="C42" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="D42" s="15" t="s">
-        <v>302</v>
-      </c>
-      <c r="E42" s="16"/>
+      <c r="D42" s="24" t="s">
+        <v>304</v>
+      </c>
+      <c r="E42" s="25"/>
     </row>
     <row r="43" spans="2:5">
       <c r="B43" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C43" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="C43" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="D43" s="15" t="s">
-        <v>302</v>
-      </c>
-      <c r="E43" s="16"/>
+      <c r="D43" s="24" t="s">
+        <v>304</v>
+      </c>
+      <c r="E43" s="25"/>
     </row>
     <row r="44" spans="2:5">
       <c r="B44" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C44" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="C44" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="D44" s="9" t="s">
-        <v>301</v>
+      <c r="D44" s="9">
+        <v>11</v>
       </c>
       <c r="E44" s="10"/>
     </row>
     <row r="45" spans="2:5">
       <c r="B45" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C45" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="C45" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="D45" s="15" t="s">
-        <v>302</v>
-      </c>
-      <c r="E45" s="16"/>
+      <c r="D45" s="24" t="s">
+        <v>304</v>
+      </c>
+      <c r="E45" s="25"/>
     </row>
     <row r="46" spans="2:5">
       <c r="B46" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D46" s="17"/>
-      <c r="E46" s="18"/>
+        <v>68</v>
+      </c>
+      <c r="D46" s="22"/>
+      <c r="E46" s="23"/>
     </row>
     <row r="47" spans="2:5">
       <c r="B47" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="D47" s="9" t="s">
-        <v>301</v>
+        <v>70</v>
+      </c>
+      <c r="D47" s="9">
+        <v>12</v>
       </c>
       <c r="E47" s="10"/>
     </row>
     <row r="48" spans="2:5">
       <c r="B48" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C48" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D48" s="15" t="s">
-        <v>302</v>
-      </c>
-      <c r="E48" s="16"/>
+        <v>0</v>
+      </c>
+      <c r="D48" s="24" t="s">
+        <v>304</v>
+      </c>
+      <c r="E48" s="25"/>
     </row>
     <row r="49" spans="2:5">
       <c r="B49" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C49" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="C49" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="D49" s="9" t="s">
-        <v>301</v>
+      <c r="D49" s="9">
+        <v>13</v>
       </c>
       <c r="E49" s="10"/>
     </row>
     <row r="50" spans="2:5">
       <c r="B50" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C50" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="C50" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="D50" s="9" t="s">
-        <v>301</v>
+      <c r="D50" s="9">
+        <v>14</v>
       </c>
       <c r="E50" s="10"/>
     </row>
     <row r="51" spans="2:5">
       <c r="B51" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C51" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="C51" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="D51" s="9" t="s">
-        <v>301</v>
+      <c r="D51" s="9">
+        <v>15</v>
       </c>
       <c r="E51" s="10"/>
     </row>
     <row r="52" spans="2:5">
       <c r="B52" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="D52" s="15" t="s">
-        <v>302</v>
-      </c>
-      <c r="E52" s="16"/>
+        <v>0</v>
+      </c>
+      <c r="D52" s="24" t="s">
+        <v>304</v>
+      </c>
+      <c r="E52" s="25"/>
     </row>
     <row r="53" spans="2:5">
       <c r="B53" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C53" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="C53" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="D53" s="9" t="s">
-        <v>301</v>
+      <c r="D53" s="9">
+        <v>16</v>
       </c>
       <c r="E53" s="10"/>
     </row>
     <row r="54" spans="2:5">
       <c r="B54" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="D54" s="15" t="s">
-        <v>302</v>
-      </c>
-      <c r="E54" s="16"/>
+        <v>0</v>
+      </c>
+      <c r="D54" s="24" t="s">
+        <v>304</v>
+      </c>
+      <c r="E54" s="25"/>
     </row>
     <row r="55" spans="2:5">
       <c r="B55" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C55" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="C55" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="D55" s="9" t="s">
-        <v>301</v>
+      <c r="D55" s="9">
+        <v>17</v>
       </c>
       <c r="E55" s="10"/>
     </row>
     <row r="56" spans="2:5">
       <c r="B56" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C56" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="C56" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="D56" s="9" t="s">
-        <v>301</v>
+      <c r="D56" s="9">
+        <v>18</v>
       </c>
       <c r="E56" s="10"/>
     </row>
     <row r="57" spans="2:5">
       <c r="B57" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C57" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C57" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="D57" s="19"/>
-      <c r="E57" s="20"/>
+      <c r="D57" s="16"/>
+      <c r="E57" s="17"/>
     </row>
     <row r="58" spans="2:5">
       <c r="B58" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="D58" s="23"/>
-      <c r="E58" s="24"/>
+        <v>87</v>
+      </c>
+      <c r="D58" s="18"/>
+      <c r="E58" s="19"/>
     </row>
     <row r="59" spans="2:5">
       <c r="B59" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="D59" s="21"/>
-      <c r="E59" s="22"/>
+        <v>88</v>
+      </c>
+      <c r="D59" s="20"/>
+      <c r="E59" s="21"/>
     </row>
     <row r="60" spans="2:5">
       <c r="B60" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C60" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="C60" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="D60" s="15" t="s">
-        <v>302</v>
-      </c>
-      <c r="E60" s="16"/>
+      <c r="D60" s="24" t="s">
+        <v>304</v>
+      </c>
+      <c r="E60" s="25"/>
     </row>
     <row r="61" spans="2:5">
       <c r="B61" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="C61" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="C61" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="D61" s="15" t="s">
-        <v>302</v>
-      </c>
-      <c r="E61" s="16"/>
+      <c r="D61" s="24" t="s">
+        <v>304</v>
+      </c>
+      <c r="E61" s="25"/>
     </row>
     <row r="62" spans="2:5">
       <c r="B62" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D62" s="32"/>
-      <c r="E62" s="33"/>
+        <v>0</v>
+      </c>
+      <c r="D62" s="31"/>
+      <c r="E62" s="32"/>
     </row>
     <row r="63" spans="2:5">
       <c r="B63" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C63" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C63" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="D63" s="34"/>
-      <c r="E63" s="35"/>
+      <c r="D63" s="33"/>
+      <c r="E63" s="34"/>
     </row>
     <row r="64" spans="2:5">
       <c r="B64" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="C64" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="C64" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="D64" s="9" t="s">
-        <v>301</v>
+      <c r="D64" s="9">
+        <v>19</v>
       </c>
       <c r="E64" s="10" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
     </row>
     <row r="65" spans="2:5">
       <c r="B65" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="C65" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="C65" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="D65" s="9" t="s">
-        <v>301</v>
+      <c r="D65" s="9">
+        <v>20</v>
       </c>
       <c r="E65" s="10"/>
     </row>
     <row r="66" spans="2:5">
       <c r="B66" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="C66" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="C66" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="D66" s="9" t="s">
-        <v>301</v>
+      <c r="D66" s="9">
+        <v>21</v>
       </c>
       <c r="E66" s="10"/>
     </row>
     <row r="67" spans="2:5">
       <c r="B67" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="C67" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="C67" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="D67" s="9" t="s">
-        <v>301</v>
+      <c r="D67" s="9">
+        <v>22</v>
       </c>
       <c r="E67" s="10"/>
     </row>
     <row r="68" spans="2:5">
       <c r="B68" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="C68" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="C68" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="D68" s="15" t="s">
-        <v>302</v>
-      </c>
-      <c r="E68" s="16"/>
+      <c r="D68" s="24" t="s">
+        <v>304</v>
+      </c>
+      <c r="E68" s="25"/>
     </row>
     <row r="69" spans="2:5">
       <c r="B69" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="C69" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="C69" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="D69" s="15" t="s">
-        <v>302</v>
-      </c>
-      <c r="E69" s="16"/>
+      <c r="D69" s="24" t="s">
+        <v>304</v>
+      </c>
+      <c r="E69" s="25"/>
     </row>
     <row r="70" spans="2:5">
       <c r="B70" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C70" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="C70" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="D70" s="19"/>
-      <c r="E70" s="20"/>
+      <c r="D70" s="16"/>
+      <c r="E70" s="17"/>
     </row>
     <row r="71" spans="2:5">
       <c r="B71" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C71" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="C71" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="D71" s="21"/>
-      <c r="E71" s="22"/>
+      <c r="D71" s="20"/>
+      <c r="E71" s="21"/>
     </row>
     <row r="72" spans="2:5">
       <c r="B72" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="C72" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="C72" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="D72" s="15" t="s">
-        <v>302</v>
-      </c>
-      <c r="E72" s="16"/>
+      <c r="D72" s="24" t="s">
+        <v>304</v>
+      </c>
+      <c r="E72" s="25"/>
     </row>
     <row r="73" spans="2:5">
       <c r="B73" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D73" s="19"/>
-      <c r="E73" s="20"/>
+        <v>0</v>
+      </c>
+      <c r="D73" s="16"/>
+      <c r="E73" s="17"/>
     </row>
     <row r="74" spans="2:5">
       <c r="B74" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D74" s="23"/>
-      <c r="E74" s="24"/>
+        <v>0</v>
+      </c>
+      <c r="D74" s="18"/>
+      <c r="E74" s="19"/>
     </row>
     <row r="75" spans="2:5">
       <c r="B75" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C75" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="C75" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="D75" s="23"/>
-      <c r="E75" s="24"/>
+      <c r="D75" s="18"/>
+      <c r="E75" s="19"/>
     </row>
     <row r="76" spans="2:5">
       <c r="B76" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="C76" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="C76" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="D76" s="23"/>
-      <c r="E76" s="24"/>
+      <c r="D76" s="18"/>
+      <c r="E76" s="19"/>
     </row>
     <row r="77" spans="2:5">
       <c r="B77" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="D77" s="21"/>
-      <c r="E77" s="22"/>
+        <v>120</v>
+      </c>
+      <c r="D77" s="20"/>
+      <c r="E77" s="21"/>
     </row>
     <row r="78" spans="2:5">
       <c r="B78" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="C78" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="C78" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="D78" s="9" t="s">
-        <v>301</v>
+      <c r="D78" s="9">
+        <v>23</v>
       </c>
       <c r="E78" s="10"/>
     </row>
     <row r="79" spans="2:5">
       <c r="B79" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="C79" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="C79" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="D79" s="9" t="s">
-        <v>301</v>
+      <c r="D79" s="9">
+        <v>24</v>
       </c>
       <c r="E79" s="10"/>
     </row>
     <row r="80" spans="2:5">
       <c r="B80" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C80" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="C80" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="D80" s="9" t="s">
-        <v>301</v>
+      <c r="D80" s="9">
+        <v>25</v>
       </c>
       <c r="E80" s="10"/>
     </row>
     <row r="81" spans="2:5">
       <c r="B81" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="C81" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="C81" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="D81" s="9" t="s">
-        <v>301</v>
+      <c r="D81" s="9">
+        <v>26</v>
       </c>
       <c r="E81" s="10"/>
     </row>
     <row r="82" spans="2:5">
       <c r="B82" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="D82" s="17"/>
-      <c r="E82" s="18"/>
+        <v>129</v>
+      </c>
+      <c r="D82" s="22"/>
+      <c r="E82" s="23"/>
     </row>
     <row r="83" spans="2:5">
       <c r="B83" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="C83" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="C83" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="D83" s="9" t="s">
-        <v>301</v>
+      <c r="D83" s="9">
+        <v>27</v>
       </c>
       <c r="E83" s="10"/>
     </row>
     <row r="84" spans="2:5">
       <c r="B84" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="D84" s="19"/>
-      <c r="E84" s="27"/>
+        <v>132</v>
+      </c>
+      <c r="D84" s="16"/>
+      <c r="E84" s="26"/>
     </row>
     <row r="85" spans="2:5">
       <c r="B85" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="D85" s="28"/>
-      <c r="E85" s="29"/>
+        <v>133</v>
+      </c>
+      <c r="D85" s="27"/>
+      <c r="E85" s="28"/>
     </row>
     <row r="86" spans="2:5">
       <c r="B86" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="D86" s="30"/>
-      <c r="E86" s="31"/>
+        <v>134</v>
+      </c>
+      <c r="D86" s="29"/>
+      <c r="E86" s="30"/>
     </row>
     <row r="87" spans="2:5">
       <c r="B87" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="C87" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="C87" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="D87" s="9" t="s">
-        <v>301</v>
+      <c r="D87" s="9">
+        <v>28</v>
       </c>
       <c r="E87" s="10"/>
     </row>
     <row r="88" spans="2:5">
       <c r="B88" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="C88" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="C88" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="D88" s="9" t="s">
-        <v>301</v>
+      <c r="D88" s="9">
+        <v>29</v>
       </c>
       <c r="E88" s="10"/>
     </row>
     <row r="89" spans="2:5">
       <c r="B89" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="D89" s="19"/>
-      <c r="E89" s="20"/>
+        <v>139</v>
+      </c>
+      <c r="D89" s="16"/>
+      <c r="E89" s="17"/>
     </row>
     <row r="90" spans="2:5">
       <c r="B90" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="C90" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="C90" s="13" t="s">
-        <v>142</v>
-      </c>
-      <c r="D90" s="21"/>
-      <c r="E90" s="22"/>
+      <c r="D90" s="20"/>
+      <c r="E90" s="21"/>
     </row>
     <row r="91" spans="2:5">
       <c r="B91" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="C91" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="C91" s="8" t="s">
-        <v>144</v>
-      </c>
-      <c r="D91" s="15" t="s">
-        <v>302</v>
-      </c>
-      <c r="E91" s="16"/>
+      <c r="D91" s="24" t="s">
+        <v>304</v>
+      </c>
+      <c r="E91" s="25"/>
     </row>
     <row r="92" spans="2:5">
       <c r="B92" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D92" s="19"/>
-      <c r="E92" s="20"/>
+        <v>0</v>
+      </c>
+      <c r="D92" s="16"/>
+      <c r="E92" s="17"/>
     </row>
     <row r="93" spans="2:5">
       <c r="B93" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="D93" s="23"/>
-      <c r="E93" s="24"/>
+        <v>145</v>
+      </c>
+      <c r="D93" s="18"/>
+      <c r="E93" s="19"/>
     </row>
     <row r="94" spans="2:5">
       <c r="B94" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C94" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="C94" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="D94" s="23"/>
-      <c r="E94" s="24"/>
+      <c r="D94" s="18"/>
+      <c r="E94" s="19"/>
     </row>
     <row r="95" spans="2:5">
       <c r="B95" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C95" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="C95" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="D95" s="23"/>
-      <c r="E95" s="24"/>
+      <c r="D95" s="18"/>
+      <c r="E95" s="19"/>
     </row>
     <row r="96" spans="2:5">
       <c r="B96" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C96" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="C96" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="D96" s="23"/>
-      <c r="E96" s="24"/>
+      <c r="D96" s="18"/>
+      <c r="E96" s="19"/>
     </row>
     <row r="97" spans="2:5">
       <c r="B97" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C97" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="C97" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="D97" s="23"/>
-      <c r="E97" s="24"/>
+      <c r="D97" s="18"/>
+      <c r="E97" s="19"/>
     </row>
     <row r="98" spans="2:5">
       <c r="B98" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C98" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="C98" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="D98" s="23"/>
-      <c r="E98" s="24"/>
+      <c r="D98" s="18"/>
+      <c r="E98" s="19"/>
     </row>
     <row r="99" spans="2:5">
       <c r="B99" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C99" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="C99" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="D99" s="23"/>
-      <c r="E99" s="24"/>
+      <c r="D99" s="18"/>
+      <c r="E99" s="19"/>
     </row>
     <row r="100" spans="2:5">
       <c r="B100" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C100" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="C100" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="D100" s="23"/>
-      <c r="E100" s="24"/>
+      <c r="D100" s="18"/>
+      <c r="E100" s="19"/>
     </row>
     <row r="101" spans="2:5">
       <c r="B101" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C101" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="C101" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="D101" s="23"/>
-      <c r="E101" s="24"/>
+      <c r="D101" s="18"/>
+      <c r="E101" s="19"/>
     </row>
     <row r="102" spans="2:5">
       <c r="B102" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C102" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="C102" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="D102" s="23"/>
-      <c r="E102" s="24"/>
+      <c r="D102" s="18"/>
+      <c r="E102" s="19"/>
     </row>
     <row r="103" spans="2:5">
       <c r="B103" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C103" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="C103" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="D103" s="23"/>
-      <c r="E103" s="24"/>
+      <c r="D103" s="18"/>
+      <c r="E103" s="19"/>
     </row>
     <row r="104" spans="2:5">
       <c r="B104" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C104" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="C104" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="D104" s="23"/>
-      <c r="E104" s="24"/>
+      <c r="D104" s="18"/>
+      <c r="E104" s="19"/>
     </row>
     <row r="105" spans="2:5">
       <c r="B105" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C105" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="C105" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="D105" s="23"/>
-      <c r="E105" s="24"/>
+      <c r="D105" s="18"/>
+      <c r="E105" s="19"/>
     </row>
     <row r="106" spans="2:5">
       <c r="B106" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C106" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="C106" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="D106" s="23"/>
-      <c r="E106" s="24"/>
+      <c r="D106" s="18"/>
+      <c r="E106" s="19"/>
     </row>
     <row r="107" spans="2:5">
       <c r="B107" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="C107" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="C107" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="D107" s="23"/>
-      <c r="E107" s="24"/>
+      <c r="D107" s="18"/>
+      <c r="E107" s="19"/>
     </row>
     <row r="108" spans="2:5">
       <c r="B108" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C108" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="C108" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="D108" s="23"/>
-      <c r="E108" s="24"/>
+      <c r="D108" s="18"/>
+      <c r="E108" s="19"/>
     </row>
     <row r="109" spans="2:5">
       <c r="B109" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="C109" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="C109" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="D109" s="23"/>
-      <c r="E109" s="24"/>
+      <c r="D109" s="18"/>
+      <c r="E109" s="19"/>
     </row>
     <row r="110" spans="2:5">
       <c r="B110" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C110" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="C110" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="D110" s="23"/>
-      <c r="E110" s="24"/>
+      <c r="D110" s="18"/>
+      <c r="E110" s="19"/>
     </row>
     <row r="111" spans="2:5">
       <c r="B111" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D111" s="23"/>
-      <c r="E111" s="24"/>
+        <v>0</v>
+      </c>
+      <c r="D111" s="18"/>
+      <c r="E111" s="19"/>
     </row>
     <row r="112" spans="2:5">
       <c r="B112" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D112" s="23"/>
-      <c r="E112" s="24"/>
+        <v>0</v>
+      </c>
+      <c r="D112" s="18"/>
+      <c r="E112" s="19"/>
     </row>
     <row r="113" spans="2:5">
       <c r="B113" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="C113" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="C113" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="D113" s="23"/>
-      <c r="E113" s="24"/>
+      <c r="D113" s="18"/>
+      <c r="E113" s="19"/>
     </row>
     <row r="114" spans="2:5">
       <c r="B114" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="D114" s="23"/>
-      <c r="E114" s="24"/>
+        <v>184</v>
+      </c>
+      <c r="D114" s="18"/>
+      <c r="E114" s="19"/>
     </row>
     <row r="115" spans="2:5">
       <c r="B115" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D115" s="23"/>
-      <c r="E115" s="24"/>
+        <v>0</v>
+      </c>
+      <c r="D115" s="18"/>
+      <c r="E115" s="19"/>
     </row>
     <row r="116" spans="2:5">
       <c r="B116" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D116" s="23"/>
-      <c r="E116" s="24"/>
+        <v>0</v>
+      </c>
+      <c r="D116" s="18"/>
+      <c r="E116" s="19"/>
     </row>
     <row r="117" spans="2:5">
       <c r="B117" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="D117" s="23"/>
-      <c r="E117" s="24"/>
+        <v>187</v>
+      </c>
+      <c r="D117" s="18"/>
+      <c r="E117" s="19"/>
     </row>
     <row r="118" spans="2:5">
       <c r="B118" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="D118" s="23"/>
-      <c r="E118" s="24"/>
+        <v>188</v>
+      </c>
+      <c r="D118" s="18"/>
+      <c r="E118" s="19"/>
     </row>
     <row r="119" spans="2:5">
       <c r="B119" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D119" s="23"/>
-      <c r="E119" s="24"/>
+        <v>0</v>
+      </c>
+      <c r="D119" s="18"/>
+      <c r="E119" s="19"/>
     </row>
     <row r="120" spans="2:5">
       <c r="B120" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="C120" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="C120" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="D120" s="23"/>
-      <c r="E120" s="24"/>
+      <c r="D120" s="18"/>
+      <c r="E120" s="19"/>
     </row>
     <row r="121" spans="2:5">
       <c r="B121" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="C121" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="C121" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="D121" s="23"/>
-      <c r="E121" s="24"/>
+      <c r="D121" s="18"/>
+      <c r="E121" s="19"/>
     </row>
     <row r="122" spans="2:5">
       <c r="B122" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="C122" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="C122" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="D122" s="23"/>
-      <c r="E122" s="24"/>
+      <c r="D122" s="18"/>
+      <c r="E122" s="19"/>
     </row>
     <row r="123" spans="2:5">
       <c r="B123" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="D123" s="21"/>
-      <c r="E123" s="22"/>
+        <v>196</v>
+      </c>
+      <c r="D123" s="20"/>
+      <c r="E123" s="21"/>
     </row>
     <row r="124" spans="2:5">
       <c r="B124" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="C124" s="8" t="s">
         <v>198</v>
       </c>
-      <c r="C124" s="8" t="s">
-        <v>199</v>
-      </c>
-      <c r="D124" s="14" t="s">
-        <v>301</v>
+      <c r="D124" s="36">
+        <v>30</v>
       </c>
       <c r="E124" s="10"/>
     </row>
     <row r="125" spans="2:5">
       <c r="B125" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="C125" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="C125" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="D125" s="17"/>
-      <c r="E125" s="18"/>
+      <c r="D125" s="22"/>
+      <c r="E125" s="23"/>
     </row>
     <row r="126" spans="2:5">
       <c r="B126" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="C126" s="8" t="s">
         <v>202</v>
       </c>
-      <c r="C126" s="8" t="s">
-        <v>203</v>
-      </c>
-      <c r="D126" s="9" t="s">
-        <v>301</v>
+      <c r="D126" s="9">
+        <v>31</v>
       </c>
       <c r="E126" s="10"/>
     </row>
     <row r="127" spans="2:5">
       <c r="B127" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="D127" s="19"/>
-      <c r="E127" s="20"/>
+        <v>203</v>
+      </c>
+      <c r="D127" s="16"/>
+      <c r="E127" s="17"/>
     </row>
     <row r="128" spans="2:5">
       <c r="B128" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C128" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="D128" s="20"/>
+      <c r="E128" s="21"/>
+    </row>
+    <row r="129" spans="2:5">
+      <c r="B129" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C129" s="8" t="s">
         <v>205</v>
       </c>
-      <c r="D128" s="23"/>
-      <c r="E128" s="24"/>
-    </row>
-    <row r="129" spans="2:5">
-      <c r="B129" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C129" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="D129" s="23"/>
-      <c r="E129" s="24"/>
+      <c r="D129" s="35">
+        <v>32</v>
+      </c>
+      <c r="E129" s="35" t="s">
+        <v>301</v>
+      </c>
     </row>
     <row r="130" spans="2:5">
       <c r="B130" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D130" s="23"/>
-      <c r="E130" s="24"/>
+        <v>0</v>
+      </c>
+      <c r="D130" s="16"/>
+      <c r="E130" s="17"/>
     </row>
     <row r="131" spans="2:5">
       <c r="B131" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="D131" s="23"/>
-      <c r="E131" s="24"/>
+        <v>207</v>
+      </c>
+      <c r="D131" s="18"/>
+      <c r="E131" s="19"/>
     </row>
     <row r="132" spans="2:5">
       <c r="B132" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="C132" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="C132" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="D132" s="23"/>
-      <c r="E132" s="24"/>
+      <c r="D132" s="18"/>
+      <c r="E132" s="19"/>
     </row>
     <row r="133" spans="2:5">
       <c r="B133" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="D133" s="23"/>
-      <c r="E133" s="24"/>
+        <v>210</v>
+      </c>
+      <c r="D133" s="18"/>
+      <c r="E133" s="19"/>
     </row>
     <row r="134" spans="2:5">
       <c r="B134" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D134" s="23"/>
-      <c r="E134" s="24"/>
+        <v>0</v>
+      </c>
+      <c r="D134" s="18"/>
+      <c r="E134" s="19"/>
     </row>
     <row r="135" spans="2:5">
       <c r="B135" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="C135" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="C135" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="D135" s="23"/>
-      <c r="E135" s="24"/>
+      <c r="D135" s="18"/>
+      <c r="E135" s="19"/>
     </row>
     <row r="136" spans="2:5">
       <c r="B136" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="D136" s="23"/>
-      <c r="E136" s="24"/>
+        <v>214</v>
+      </c>
+      <c r="D136" s="18"/>
+      <c r="E136" s="19"/>
     </row>
     <row r="137" spans="2:5">
       <c r="B137" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="C137" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="C137" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="D137" s="23"/>
-      <c r="E137" s="24"/>
+      <c r="D137" s="18"/>
+      <c r="E137" s="19"/>
     </row>
     <row r="138" spans="2:5">
       <c r="B138" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="C138" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="C138" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="D138" s="23"/>
-      <c r="E138" s="24"/>
+      <c r="D138" s="18"/>
+      <c r="E138" s="19"/>
     </row>
     <row r="139" spans="2:5">
       <c r="B139" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="C139" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="C139" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="D139" s="23"/>
-      <c r="E139" s="24"/>
+      <c r="D139" s="18"/>
+      <c r="E139" s="19"/>
     </row>
     <row r="140" spans="2:5">
       <c r="B140" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="D140" s="23"/>
-      <c r="E140" s="24"/>
+        <v>221</v>
+      </c>
+      <c r="D140" s="18"/>
+      <c r="E140" s="19"/>
     </row>
     <row r="141" spans="2:5">
       <c r="B141" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="D141" s="23"/>
-      <c r="E141" s="24"/>
+        <v>222</v>
+      </c>
+      <c r="D141" s="18"/>
+      <c r="E141" s="19"/>
     </row>
     <row r="142" spans="2:5">
       <c r="B142" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="D142" s="23"/>
-      <c r="E142" s="24"/>
+        <v>223</v>
+      </c>
+      <c r="D142" s="18"/>
+      <c r="E142" s="19"/>
     </row>
     <row r="143" spans="2:5">
       <c r="B143" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="C143" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="C143" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="D143" s="23"/>
-      <c r="E143" s="24"/>
+      <c r="D143" s="18"/>
+      <c r="E143" s="19"/>
     </row>
     <row r="144" spans="2:5">
       <c r="B144" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D144" s="23"/>
-      <c r="E144" s="24"/>
+        <v>0</v>
+      </c>
+      <c r="D144" s="18"/>
+      <c r="E144" s="19"/>
     </row>
     <row r="145" spans="2:5">
       <c r="B145" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="C145" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="C145" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="D145" s="23"/>
-      <c r="E145" s="24"/>
+      <c r="D145" s="18"/>
+      <c r="E145" s="19"/>
     </row>
     <row r="146" spans="2:5">
       <c r="B146" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="C146" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="C146" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="D146" s="23"/>
-      <c r="E146" s="24"/>
+      <c r="D146" s="18"/>
+      <c r="E146" s="19"/>
     </row>
     <row r="147" spans="2:5">
       <c r="B147" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="C147" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="C147" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="D147" s="23"/>
-      <c r="E147" s="24"/>
+      <c r="D147" s="18"/>
+      <c r="E147" s="19"/>
     </row>
     <row r="148" spans="2:5">
       <c r="B148" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="D148" s="23"/>
-      <c r="E148" s="24"/>
+        <v>233</v>
+      </c>
+      <c r="D148" s="18"/>
+      <c r="E148" s="19"/>
     </row>
     <row r="149" spans="2:5">
       <c r="B149" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="C149" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="C149" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="D149" s="23"/>
-      <c r="E149" s="24"/>
+      <c r="D149" s="18"/>
+      <c r="E149" s="19"/>
     </row>
     <row r="150" spans="2:5">
       <c r="B150" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C150" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="C150" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="D150" s="23"/>
-      <c r="E150" s="24"/>
+      <c r="D150" s="18"/>
+      <c r="E150" s="19"/>
     </row>
     <row r="151" spans="2:5">
       <c r="B151" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D151" s="21"/>
-      <c r="E151" s="22"/>
+        <v>0</v>
+      </c>
+      <c r="D151" s="20"/>
+      <c r="E151" s="21"/>
     </row>
     <row r="152" spans="2:5">
       <c r="B152" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="C152" s="8" t="s">
         <v>240</v>
       </c>
-      <c r="C152" s="8" t="s">
-        <v>241</v>
-      </c>
-      <c r="D152" s="15" t="s">
-        <v>302</v>
-      </c>
-      <c r="E152" s="16"/>
+      <c r="D152" s="24" t="s">
+        <v>304</v>
+      </c>
+      <c r="E152" s="25"/>
     </row>
     <row r="153" spans="2:5">
       <c r="B153" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="C153" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="C153" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="D153" s="19"/>
-      <c r="E153" s="20"/>
+      <c r="D153" s="16"/>
+      <c r="E153" s="17"/>
     </row>
     <row r="154" spans="2:5">
       <c r="B154" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="C154" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="C154" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="D154" s="23"/>
-      <c r="E154" s="24"/>
+      <c r="D154" s="18"/>
+      <c r="E154" s="19"/>
     </row>
     <row r="155" spans="2:5">
       <c r="B155" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="C155" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="C155" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="D155" s="23"/>
-      <c r="E155" s="24"/>
+      <c r="D155" s="18"/>
+      <c r="E155" s="19"/>
     </row>
     <row r="156" spans="2:5">
       <c r="B156" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="C156" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="C156" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="D156" s="23"/>
-      <c r="E156" s="24"/>
+      <c r="D156" s="18"/>
+      <c r="E156" s="19"/>
     </row>
     <row r="157" spans="2:5">
       <c r="B157" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="C157" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="C157" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="D157" s="23"/>
-      <c r="E157" s="24"/>
+      <c r="D157" s="18"/>
+      <c r="E157" s="19"/>
     </row>
     <row r="158" spans="2:5">
       <c r="B158" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="C158" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="C158" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="D158" s="23"/>
-      <c r="E158" s="24"/>
+      <c r="D158" s="18"/>
+      <c r="E158" s="19"/>
     </row>
     <row r="159" spans="2:5">
       <c r="B159" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="C159" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="C159" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="D159" s="23"/>
-      <c r="E159" s="24"/>
+      <c r="D159" s="18"/>
+      <c r="E159" s="19"/>
     </row>
     <row r="160" spans="2:5">
       <c r="B160" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="C160" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="C160" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="D160" s="23"/>
-      <c r="E160" s="24"/>
+      <c r="D160" s="18"/>
+      <c r="E160" s="19"/>
     </row>
     <row r="161" spans="2:5">
       <c r="B161" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D161" s="21"/>
-      <c r="E161" s="22"/>
+        <v>0</v>
+      </c>
+      <c r="D161" s="20"/>
+      <c r="E161" s="21"/>
     </row>
     <row r="162" spans="2:5">
       <c r="B162" s="8" t="s">
+        <v>258</v>
+      </c>
+      <c r="C162" s="8" t="s">
         <v>259</v>
       </c>
-      <c r="C162" s="8" t="s">
-        <v>260</v>
-      </c>
-      <c r="D162" s="9" t="s">
-        <v>301</v>
+      <c r="D162" s="9">
+        <v>33</v>
       </c>
       <c r="E162" s="10"/>
     </row>
     <row r="163" spans="2:5">
       <c r="B163" s="8" t="s">
+        <v>260</v>
+      </c>
+      <c r="C163" s="8" t="s">
         <v>261</v>
       </c>
-      <c r="C163" s="8" t="s">
-        <v>262</v>
-      </c>
-      <c r="D163" s="15" t="s">
-        <v>302</v>
-      </c>
-      <c r="E163" s="16"/>
+      <c r="D163" s="24" t="s">
+        <v>304</v>
+      </c>
+      <c r="E163" s="25"/>
     </row>
     <row r="164" spans="2:5">
       <c r="B164" s="8" t="s">
+        <v>262</v>
+      </c>
+      <c r="C164" s="8" t="s">
         <v>263</v>
       </c>
-      <c r="C164" s="8" t="s">
-        <v>264</v>
-      </c>
-      <c r="D164" s="9" t="s">
-        <v>301</v>
+      <c r="D164" s="9">
+        <v>34</v>
       </c>
       <c r="E164" s="10"/>
     </row>
     <row r="165" spans="2:5">
       <c r="B165" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="C165" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="C165" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="D165" s="19"/>
-      <c r="E165" s="20"/>
+      <c r="D165" s="16"/>
+      <c r="E165" s="17"/>
     </row>
     <row r="166" spans="2:5">
       <c r="B166" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="C166" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="C166" s="2" t="s">
-        <v>268</v>
-      </c>
-      <c r="D166" s="23"/>
-      <c r="E166" s="24"/>
+      <c r="D166" s="18"/>
+      <c r="E166" s="19"/>
     </row>
     <row r="167" spans="2:5">
       <c r="B167" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="C167" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="C167" s="2" t="s">
-        <v>270</v>
-      </c>
-      <c r="D167" s="23"/>
-      <c r="E167" s="24"/>
+      <c r="D167" s="18"/>
+      <c r="E167" s="19"/>
     </row>
     <row r="168" spans="2:5">
       <c r="B168" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="C168" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="C168" s="2" t="s">
-        <v>272</v>
-      </c>
-      <c r="D168" s="23"/>
-      <c r="E168" s="24"/>
+      <c r="D168" s="18"/>
+      <c r="E168" s="19"/>
     </row>
     <row r="169" spans="2:5">
       <c r="B169" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="C169" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="C169" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="D169" s="23"/>
-      <c r="E169" s="24"/>
+      <c r="D169" s="18"/>
+      <c r="E169" s="19"/>
     </row>
     <row r="170" spans="2:5">
       <c r="B170" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="C170" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="C170" s="2" t="s">
-        <v>276</v>
-      </c>
-      <c r="D170" s="23"/>
-      <c r="E170" s="24"/>
+      <c r="D170" s="18"/>
+      <c r="E170" s="19"/>
     </row>
     <row r="171" spans="2:5">
       <c r="B171" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="C171" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="C171" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="D171" s="23"/>
-      <c r="E171" s="24"/>
+      <c r="D171" s="18"/>
+      <c r="E171" s="19"/>
     </row>
     <row r="172" spans="2:5">
       <c r="B172" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="C172" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="C172" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="D172" s="23"/>
-      <c r="E172" s="24"/>
+      <c r="D172" s="18"/>
+      <c r="E172" s="19"/>
     </row>
     <row r="173" spans="2:5">
       <c r="B173" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D173" s="23"/>
-      <c r="E173" s="24"/>
+        <v>0</v>
+      </c>
+      <c r="D173" s="18"/>
+      <c r="E173" s="19"/>
     </row>
     <row r="174" spans="2:5">
       <c r="B174" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="C174" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="C174" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="D174" s="23"/>
-      <c r="E174" s="24"/>
+      <c r="D174" s="18"/>
+      <c r="E174" s="19"/>
     </row>
     <row r="175" spans="2:5">
       <c r="B175" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C175" s="2" t="s">
-        <v>284</v>
-      </c>
-      <c r="D175" s="23"/>
-      <c r="E175" s="24"/>
+        <v>283</v>
+      </c>
+      <c r="D175" s="18"/>
+      <c r="E175" s="19"/>
     </row>
     <row r="176" spans="2:5">
       <c r="B176" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C176" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="D176" s="23"/>
-      <c r="E176" s="24"/>
+        <v>284</v>
+      </c>
+      <c r="D176" s="18"/>
+      <c r="E176" s="19"/>
     </row>
     <row r="177" spans="2:5">
       <c r="B177" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C177" s="2" t="s">
-        <v>286</v>
-      </c>
-      <c r="D177" s="23"/>
-      <c r="E177" s="24"/>
+        <v>285</v>
+      </c>
+      <c r="D177" s="18"/>
+      <c r="E177" s="19"/>
     </row>
     <row r="178" spans="2:5">
       <c r="B178" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C178" s="2" t="s">
-        <v>287</v>
-      </c>
-      <c r="D178" s="23"/>
-      <c r="E178" s="24"/>
+        <v>286</v>
+      </c>
+      <c r="D178" s="18"/>
+      <c r="E178" s="19"/>
     </row>
     <row r="179" spans="2:5">
       <c r="B179" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C179" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D179" s="23"/>
-      <c r="E179" s="24"/>
+        <v>0</v>
+      </c>
+      <c r="D179" s="18"/>
+      <c r="E179" s="19"/>
     </row>
     <row r="180" spans="2:5">
       <c r="B180" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C180" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D180" s="23"/>
-      <c r="E180" s="24"/>
+        <v>0</v>
+      </c>
+      <c r="D180" s="18"/>
+      <c r="E180" s="19"/>
     </row>
     <row r="181" spans="2:5">
       <c r="B181" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C181" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D181" s="23"/>
-      <c r="E181" s="24"/>
+        <v>0</v>
+      </c>
+      <c r="D181" s="18"/>
+      <c r="E181" s="19"/>
     </row>
     <row r="182" spans="2:5">
       <c r="B182" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C182" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D182" s="23"/>
-      <c r="E182" s="24"/>
+        <v>0</v>
+      </c>
+      <c r="D182" s="18"/>
+      <c r="E182" s="19"/>
     </row>
     <row r="183" spans="2:5">
       <c r="B183" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C183" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D183" s="21"/>
-      <c r="E183" s="22"/>
+        <v>0</v>
+      </c>
+      <c r="D183" s="20"/>
+      <c r="E183" s="21"/>
     </row>
     <row r="184" spans="2:5">
       <c r="B184" s="8" t="s">
+        <v>292</v>
+      </c>
+      <c r="C184" s="8" t="s">
         <v>293</v>
       </c>
-      <c r="C184" s="8" t="s">
-        <v>294</v>
-      </c>
-      <c r="D184" s="9" t="s">
-        <v>301</v>
+      <c r="D184" s="9">
+        <v>35</v>
       </c>
       <c r="E184" s="10"/>
     </row>
     <row r="185" spans="2:5">
       <c r="B185" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="C185" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="C185" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="D185" s="19"/>
-      <c r="E185" s="20"/>
+      <c r="D185" s="16"/>
+      <c r="E185" s="17"/>
     </row>
     <row r="186" spans="2:5">
       <c r="B186" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C186" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="D186" s="21"/>
-      <c r="E186" s="22"/>
+        <v>296</v>
+      </c>
+      <c r="D186" s="20"/>
+      <c r="E186" s="21"/>
     </row>
   </sheetData>
-  <mergeCells count="40">
+  <mergeCells count="41">
+    <mergeCell ref="D72:E72"/>
+    <mergeCell ref="D69:E69"/>
+    <mergeCell ref="D91:E91"/>
+    <mergeCell ref="D152:E152"/>
+    <mergeCell ref="D163:E163"/>
+    <mergeCell ref="D70:E71"/>
+    <mergeCell ref="D127:E128"/>
+    <mergeCell ref="D130:E151"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="D68:E68"/>
+    <mergeCell ref="D185:E186"/>
+    <mergeCell ref="D73:E77"/>
+    <mergeCell ref="D89:E90"/>
+    <mergeCell ref="D92:E123"/>
+    <mergeCell ref="D125:E125"/>
+    <mergeCell ref="D153:E161"/>
+    <mergeCell ref="D165:E183"/>
+    <mergeCell ref="D82:E82"/>
+    <mergeCell ref="D84:E86"/>
+    <mergeCell ref="D57:E59"/>
+    <mergeCell ref="D62:E63"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="D8:E19"/>
     <mergeCell ref="D21:E22"/>
@@ -3578,36 +3614,6 @@
     <mergeCell ref="D33:E33"/>
     <mergeCell ref="D34:E34"/>
     <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="D68:E68"/>
-    <mergeCell ref="D185:E186"/>
-    <mergeCell ref="D73:E77"/>
-    <mergeCell ref="D89:E90"/>
-    <mergeCell ref="D92:E123"/>
-    <mergeCell ref="D125:E125"/>
-    <mergeCell ref="D127:E151"/>
-    <mergeCell ref="D153:E161"/>
-    <mergeCell ref="D165:E183"/>
-    <mergeCell ref="D82:E82"/>
-    <mergeCell ref="D84:E86"/>
-    <mergeCell ref="D57:E59"/>
-    <mergeCell ref="D62:E63"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D72:E72"/>
-    <mergeCell ref="D69:E69"/>
-    <mergeCell ref="D91:E91"/>
-    <mergeCell ref="D152:E152"/>
-    <mergeCell ref="D163:E163"/>
-    <mergeCell ref="D70:E71"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
outil conversion mis à jour
</commit_message>
<xml_diff>
--- a/migration_bdd.xlsx
+++ b/migration_bdd.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="314">
   <si>
     <t>X</t>
   </si>
@@ -933,14 +933,53 @@
     <t>SQL de CONVERSION</t>
   </si>
   <si>
-    <t>ALTER TABLE clan_data MODIFY reputation_score int(11) AFTER clan_level ;</t>
+    <t>ALTER TABLE clan_data MODIFY reputation_score int(11) NOT NULL DEFAULT 0 AFTER clan_level, DROP rank ;</t>
+  </si>
+  <si>
+    <t>ALTER TABLE `accounts`
+MODIFY `login` VARCHAR(45) NOT NULL DEFAULT '',
+MODIFY `password` VARCHAR(45),
+MODIFY `lastactive` DECIMAL(20,0),
+MODIFY `accessLevel` TINYINT NOT NULL DEFAULT 0,
+MODIFY `lastIP` CHAR(15) NULL DEFAULT NULL AFTER accessLevel,
+CHANGE `lastServerId` `lastServer` TINYINT DEFAULT 1 AFTER lastIP,
+ADD `userIP` CHAR(15) AFTER lastServer,
+ADD `pcIp` CHAR(15) DEFAULT NULL AFTER userIP,
+ADD `hop1` CHAR(15) DEFAULT NULL AFTER pcIp,
+ADD `hop2` CHAR(15) DEFAULT NULL AFTER hop1,
+ADD `hop3` CHAR(15) DEFAULT NULL AFTER hop2,
+ADD `hop4` CHAR(15) DEFAULT NULL AFTER hop3,
+DROP `birthYear`,
+DROP `birthMonth`,
+DROP `birthDay` ;</t>
+  </si>
+  <si>
+    <t>Quelques rappels :</t>
+  </si>
+  <si>
+    <t>ALTER TABLE `nom_table`</t>
+  </si>
+  <si>
+    <t>MODIFY `nom_colonne` type_colonne [AFTER autre_colonne] ==&gt; modifier [et déplacer]</t>
+  </si>
+  <si>
+    <t>CHANGE `nom_colonne1` `nom_colonne2` type_colonne [AFTER autre_colonne] ==&gt; renommer &amp; modifier [et déplacer]</t>
+  </si>
+  <si>
+    <t>ADD `nom_colonne` type_colonne [AFTER autre_colonne] ==&gt; ajouter [et placer]</t>
+  </si>
+  <si>
+    <t>DROP `nom_colonne` ==&gt; supprimer</t>
+  </si>
+  <si>
+    <t>MERCI de vous baser sur les fichiers SQL de L2J pour réaliser les SQL de CONVERSION (http://svn.assembla.com/svn/vae-soli/trunk/datapack_development/sql/)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -988,6 +1027,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1009,7 +1065,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -1217,19 +1273,96 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="4"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1245,47 +1378,44 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -1305,11 +1435,56 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1605,2015 +1780,2085 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B3:E186"/>
+  <dimension ref="B1:E193"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B43" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E65" sqref="E65"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="3" width="28.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" customWidth="1"/>
-    <col min="5" max="5" width="106.85546875" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" style="35" customWidth="1"/>
+    <col min="5" max="5" width="107.5703125" style="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:5" ht="16.5" thickBot="1">
-      <c r="B3" s="3" t="s">
+    <row r="1" spans="2:5" ht="15.75" thickBot="1"/>
+    <row r="2" spans="2:5">
+      <c r="B2" s="39" t="s">
+        <v>307</v>
+      </c>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="41"/>
+    </row>
+    <row r="3" spans="2:5">
+      <c r="B3" s="42" t="s">
+        <v>308</v>
+      </c>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="44"/>
+    </row>
+    <row r="4" spans="2:5">
+      <c r="B4" s="42" t="s">
+        <v>309</v>
+      </c>
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="44"/>
+    </row>
+    <row r="5" spans="2:5">
+      <c r="B5" s="42" t="s">
+        <v>310</v>
+      </c>
+      <c r="C5" s="43"/>
+      <c r="D5" s="43"/>
+      <c r="E5" s="44"/>
+    </row>
+    <row r="6" spans="2:5">
+      <c r="B6" s="42" t="s">
+        <v>311</v>
+      </c>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="44"/>
+    </row>
+    <row r="7" spans="2:5">
+      <c r="B7" s="42" t="s">
+        <v>312</v>
+      </c>
+      <c r="C7" s="43"/>
+      <c r="D7" s="43"/>
+      <c r="E7" s="44"/>
+    </row>
+    <row r="8" spans="2:5" ht="15.75" thickBot="1">
+      <c r="B8" s="45" t="s">
+        <v>313</v>
+      </c>
+      <c r="C8" s="46"/>
+      <c r="D8" s="46"/>
+      <c r="E8" s="47"/>
+    </row>
+    <row r="10" spans="2:5" ht="16.5" thickBot="1">
+      <c r="B10" s="38" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="4" spans="2:5" ht="16.5" thickBot="1">
-      <c r="B4" s="5" t="s">
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+    </row>
+    <row r="11" spans="2:5" ht="16.5" thickBot="1">
+      <c r="B11" s="4" t="s">
         <v>297</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C11" s="5" t="s">
         <v>298</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D11" s="6" t="s">
         <v>301</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E11" s="32" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="5" spans="2:5">
-      <c r="B5" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="4" t="s">
+    <row r="12" spans="2:5">
+      <c r="B12" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="35"/>
-      <c r="E5" s="36"/>
-    </row>
-    <row r="6" spans="2:5">
-      <c r="B6" s="8" t="s">
+      <c r="D12" s="10"/>
+      <c r="E12" s="11"/>
+    </row>
+    <row r="13" spans="2:5" ht="240">
+      <c r="B13" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C13" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D13" s="36">
         <v>1</v>
       </c>
-      <c r="E6" s="10"/>
-    </row>
-    <row r="7" spans="2:5">
-      <c r="B7" s="8" t="s">
+      <c r="E13" s="33" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5">
+      <c r="B14" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C14" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D14" s="20" t="s">
         <v>303</v>
       </c>
-      <c r="E7" s="17"/>
-    </row>
-    <row r="8" spans="2:5">
-      <c r="B8" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="19"/>
-    </row>
-    <row r="9" spans="2:5">
-      <c r="B9" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="22"/>
-      <c r="E9" s="23"/>
-    </row>
-    <row r="10" spans="2:5">
-      <c r="B10" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="22"/>
-      <c r="E10" s="23"/>
-    </row>
-    <row r="11" spans="2:5">
-      <c r="B11" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="22"/>
-      <c r="E11" s="23"/>
-    </row>
-    <row r="12" spans="2:5">
-      <c r="B12" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" s="22"/>
-      <c r="E12" s="23"/>
-    </row>
-    <row r="13" spans="2:5">
-      <c r="B13" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="22"/>
-      <c r="E13" s="23"/>
-    </row>
-    <row r="14" spans="2:5">
-      <c r="B14" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D14" s="22"/>
-      <c r="E14" s="23"/>
+      <c r="E14" s="21"/>
     </row>
     <row r="15" spans="2:5">
       <c r="B15" s="2" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D15" s="22"/>
-      <c r="E15" s="23"/>
+        <v>5</v>
+      </c>
+      <c r="D15" s="12"/>
+      <c r="E15" s="13"/>
     </row>
     <row r="16" spans="2:5">
       <c r="B16" s="2" t="s">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16" s="22"/>
-      <c r="E16" s="23"/>
+        <v>6</v>
+      </c>
+      <c r="D16" s="14"/>
+      <c r="E16" s="15"/>
     </row>
     <row r="17" spans="2:5">
       <c r="B17" s="2" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D17" s="22"/>
-      <c r="E17" s="23"/>
+        <v>8</v>
+      </c>
+      <c r="D17" s="14"/>
+      <c r="E17" s="15"/>
     </row>
     <row r="18" spans="2:5">
       <c r="B18" s="2" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D18" s="22"/>
-      <c r="E18" s="23"/>
+        <v>10</v>
+      </c>
+      <c r="D18" s="14"/>
+      <c r="E18" s="15"/>
     </row>
     <row r="19" spans="2:5">
       <c r="B19" s="2" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D19" s="20"/>
-      <c r="E19" s="21"/>
+        <v>12</v>
+      </c>
+      <c r="D19" s="14"/>
+      <c r="E19" s="15"/>
     </row>
     <row r="20" spans="2:5">
-      <c r="B20" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D20" s="9">
-        <v>2</v>
-      </c>
-      <c r="E20" s="10"/>
+      <c r="B20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" s="14"/>
+      <c r="E20" s="15"/>
     </row>
     <row r="21" spans="2:5">
       <c r="B21" s="2" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D21" s="18"/>
-      <c r="E21" s="19"/>
+        <v>0</v>
+      </c>
+      <c r="D21" s="14"/>
+      <c r="E21" s="15"/>
     </row>
     <row r="22" spans="2:5">
       <c r="B22" s="2" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D22" s="20"/>
-      <c r="E22" s="21"/>
+        <v>17</v>
+      </c>
+      <c r="D22" s="14"/>
+      <c r="E22" s="15"/>
     </row>
     <row r="23" spans="2:5">
-      <c r="B23" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D23" s="9">
-        <v>3</v>
-      </c>
-      <c r="E23" s="10"/>
+      <c r="B23" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" s="14"/>
+      <c r="E23" s="15"/>
     </row>
     <row r="24" spans="2:5">
       <c r="B24" s="2" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D24" s="24"/>
-      <c r="E24" s="25"/>
+        <v>21</v>
+      </c>
+      <c r="D24" s="14"/>
+      <c r="E24" s="15"/>
     </row>
     <row r="25" spans="2:5">
-      <c r="B25" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="D25" s="9">
-        <v>4</v>
-      </c>
-      <c r="E25" s="10"/>
+      <c r="B25" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25" s="14"/>
+      <c r="E25" s="15"/>
     </row>
     <row r="26" spans="2:5">
-      <c r="B26" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C26" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="D26" s="9">
-        <v>5</v>
-      </c>
-      <c r="E26" s="10"/>
+      <c r="B26" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D26" s="16"/>
+      <c r="E26" s="17"/>
     </row>
     <row r="27" spans="2:5">
-      <c r="B27" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D27" s="18"/>
-      <c r="E27" s="19"/>
+      <c r="B27" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D27" s="36">
+        <v>2</v>
+      </c>
+      <c r="E27" s="33"/>
     </row>
     <row r="28" spans="2:5">
       <c r="B28" s="2" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D28" s="22"/>
-      <c r="E28" s="23"/>
+        <v>28</v>
+      </c>
+      <c r="D28" s="12"/>
+      <c r="E28" s="13"/>
     </row>
     <row r="29" spans="2:5">
       <c r="B29" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D29" s="16"/>
+      <c r="E29" s="17"/>
+    </row>
+    <row r="30" spans="2:5">
+      <c r="B30" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D30" s="36">
+        <v>3</v>
+      </c>
+      <c r="E30" s="33"/>
+    </row>
+    <row r="31" spans="2:5">
+      <c r="B31" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D31" s="18"/>
+      <c r="E31" s="19"/>
+    </row>
+    <row r="32" spans="2:5">
+      <c r="B32" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D32" s="36">
+        <v>4</v>
+      </c>
+      <c r="E32" s="33"/>
+    </row>
+    <row r="33" spans="2:5">
+      <c r="B33" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D33" s="36">
+        <v>5</v>
+      </c>
+      <c r="E33" s="33"/>
+    </row>
+    <row r="34" spans="2:5">
+      <c r="B34" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D34" s="12"/>
+      <c r="E34" s="13"/>
+    </row>
+    <row r="35" spans="2:5">
+      <c r="B35" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D35" s="14"/>
+      <c r="E35" s="15"/>
+    </row>
+    <row r="36" spans="2:5">
+      <c r="B36" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C29" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D29" s="22"/>
-      <c r="E29" s="23"/>
-    </row>
-    <row r="30" spans="2:5">
-      <c r="B30" s="2" t="s">
+      <c r="C36" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D36" s="14"/>
+      <c r="E36" s="15"/>
+    </row>
+    <row r="37" spans="2:5">
+      <c r="B37" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C30" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D30" s="20"/>
-      <c r="E30" s="21"/>
-    </row>
-    <row r="31" spans="2:5">
-      <c r="B31" s="8" t="s">
+      <c r="C37" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D37" s="16"/>
+      <c r="E37" s="17"/>
+    </row>
+    <row r="38" spans="2:5">
+      <c r="B38" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="C31" s="8" t="s">
+      <c r="C38" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="D31" s="9">
+      <c r="D38" s="36">
         <v>6</v>
       </c>
-      <c r="E31" s="10"/>
-    </row>
-    <row r="32" spans="2:5">
-      <c r="B32" s="8" t="s">
+      <c r="E38" s="33"/>
+    </row>
+    <row r="39" spans="2:5">
+      <c r="B39" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="C32" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D32" s="16" t="s">
+      <c r="C39" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D39" s="20" t="s">
         <v>303</v>
       </c>
-      <c r="E32" s="17"/>
-    </row>
-    <row r="33" spans="2:5">
-      <c r="B33" s="8" t="s">
+      <c r="E39" s="21"/>
+    </row>
+    <row r="40" spans="2:5">
+      <c r="B40" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C33" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D33" s="16" t="s">
+      <c r="C40" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D40" s="20" t="s">
         <v>303</v>
       </c>
-      <c r="E33" s="17"/>
-    </row>
-    <row r="34" spans="2:5">
-      <c r="B34" s="8" t="s">
+      <c r="E40" s="21"/>
+    </row>
+    <row r="41" spans="2:5">
+      <c r="B41" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="C34" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D34" s="16" t="s">
+      <c r="C41" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D41" s="20" t="s">
         <v>303</v>
       </c>
-      <c r="E34" s="17"/>
-    </row>
-    <row r="35" spans="2:5">
-      <c r="B35" s="8" t="s">
+      <c r="E41" s="21"/>
+    </row>
+    <row r="42" spans="2:5">
+      <c r="B42" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C35" s="8" t="s">
+      <c r="C42" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="D35" s="9">
+      <c r="D42" s="36">
         <v>7</v>
       </c>
-      <c r="E35" s="10"/>
-    </row>
-    <row r="36" spans="2:5">
-      <c r="B36" s="8" t="s">
+      <c r="E42" s="33"/>
+    </row>
+    <row r="43" spans="2:5">
+      <c r="B43" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C36" s="8" t="s">
+      <c r="C43" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="D36" s="9">
+      <c r="D43" s="36">
         <v>8</v>
       </c>
-      <c r="E36" s="10"/>
-    </row>
-    <row r="37" spans="2:5">
-      <c r="B37" s="8" t="s">
+      <c r="E43" s="33"/>
+    </row>
+    <row r="44" spans="2:5">
+      <c r="B44" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="C37" s="8" t="s">
+      <c r="C44" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="D37" s="9">
+      <c r="D44" s="36">
         <v>9</v>
       </c>
-      <c r="E37" s="10"/>
-    </row>
-    <row r="38" spans="2:5">
-      <c r="B38" s="8" t="s">
+      <c r="E44" s="33"/>
+    </row>
+    <row r="45" spans="2:5">
+      <c r="B45" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="C38" s="8" t="s">
+      <c r="C45" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="D38" s="16" t="s">
+      <c r="D45" s="20" t="s">
         <v>303</v>
       </c>
-      <c r="E38" s="17"/>
-    </row>
-    <row r="39" spans="2:5">
-      <c r="B39" s="8" t="s">
+      <c r="E45" s="21"/>
+    </row>
+    <row r="46" spans="2:5">
+      <c r="B46" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="C39" s="8" t="s">
+      <c r="C46" s="7" t="s">
         <v>299</v>
       </c>
-      <c r="D39" s="9">
+      <c r="D46" s="36">
         <v>10</v>
       </c>
-      <c r="E39" s="10"/>
-    </row>
-    <row r="40" spans="2:5">
-      <c r="B40" s="8" t="s">
+      <c r="E46" s="33"/>
+    </row>
+    <row r="47" spans="2:5">
+      <c r="B47" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C40" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D40" s="16" t="s">
+      <c r="C47" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D47" s="20" t="s">
         <v>303</v>
       </c>
-      <c r="E40" s="17"/>
-    </row>
-    <row r="41" spans="2:5">
-      <c r="B41" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C41" s="2" t="s">
+      <c r="E47" s="21"/>
+    </row>
+    <row r="48" spans="2:5">
+      <c r="B48" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C48" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D41" s="24"/>
-      <c r="E41" s="25"/>
-    </row>
-    <row r="42" spans="2:5">
-      <c r="B42" s="8" t="s">
+      <c r="D48" s="18"/>
+      <c r="E48" s="19"/>
+    </row>
+    <row r="49" spans="2:5">
+      <c r="B49" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="C42" s="8" t="s">
+      <c r="C49" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="D42" s="16" t="s">
+      <c r="D49" s="20" t="s">
         <v>303</v>
       </c>
-      <c r="E42" s="17"/>
-    </row>
-    <row r="43" spans="2:5">
-      <c r="B43" s="8" t="s">
+      <c r="E49" s="21"/>
+    </row>
+    <row r="50" spans="2:5">
+      <c r="B50" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="C43" s="8" t="s">
+      <c r="C50" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="D43" s="16" t="s">
+      <c r="D50" s="20" t="s">
         <v>303</v>
       </c>
-      <c r="E43" s="17"/>
-    </row>
-    <row r="44" spans="2:5">
-      <c r="B44" s="8" t="s">
+      <c r="E50" s="21"/>
+    </row>
+    <row r="51" spans="2:5">
+      <c r="B51" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="C44" s="8" t="s">
+      <c r="C51" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="D44" s="9">
+      <c r="D51" s="36">
         <v>11</v>
       </c>
-      <c r="E44" s="10"/>
-    </row>
-    <row r="45" spans="2:5">
-      <c r="B45" s="8" t="s">
+      <c r="E51" s="33"/>
+    </row>
+    <row r="52" spans="2:5">
+      <c r="B52" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="C45" s="8" t="s">
+      <c r="C52" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="D45" s="16" t="s">
+      <c r="D52" s="20" t="s">
         <v>303</v>
       </c>
-      <c r="E45" s="17"/>
-    </row>
-    <row r="46" spans="2:5">
-      <c r="B46" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C46" s="2" t="s">
+      <c r="E52" s="21"/>
+    </row>
+    <row r="53" spans="2:5">
+      <c r="B53" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C53" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D46" s="24"/>
-      <c r="E46" s="25"/>
-    </row>
-    <row r="47" spans="2:5">
-      <c r="B47" s="8" t="s">
+      <c r="D53" s="18"/>
+      <c r="E53" s="19"/>
+    </row>
+    <row r="54" spans="2:5">
+      <c r="B54" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="C47" s="8" t="s">
+      <c r="C54" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="D47" s="9">
+      <c r="D54" s="36">
         <v>12</v>
       </c>
-      <c r="E47" s="10"/>
-    </row>
-    <row r="48" spans="2:5">
-      <c r="B48" s="8" t="s">
+      <c r="E54" s="33"/>
+    </row>
+    <row r="55" spans="2:5">
+      <c r="B55" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="C48" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D48" s="16" t="s">
+      <c r="C55" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D55" s="20" t="s">
         <v>303</v>
       </c>
-      <c r="E48" s="17"/>
-    </row>
-    <row r="49" spans="2:5">
-      <c r="B49" s="8" t="s">
+      <c r="E55" s="21"/>
+    </row>
+    <row r="56" spans="2:5">
+      <c r="B56" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C49" s="8" t="s">
+      <c r="C56" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="D49" s="9">
+      <c r="D56" s="36">
         <v>13</v>
       </c>
-      <c r="E49" s="10"/>
-    </row>
-    <row r="50" spans="2:5">
-      <c r="B50" s="8" t="s">
+      <c r="E56" s="33"/>
+    </row>
+    <row r="57" spans="2:5">
+      <c r="B57" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="C50" s="8" t="s">
+      <c r="C57" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="D50" s="9">
+      <c r="D57" s="36">
         <v>14</v>
       </c>
-      <c r="E50" s="10"/>
-    </row>
-    <row r="51" spans="2:5">
-      <c r="B51" s="8" t="s">
+      <c r="E57" s="33"/>
+    </row>
+    <row r="58" spans="2:5">
+      <c r="B58" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="C51" s="8" t="s">
+      <c r="C58" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="D51" s="9">
+      <c r="D58" s="36">
         <v>15</v>
       </c>
-      <c r="E51" s="10"/>
-    </row>
-    <row r="52" spans="2:5">
-      <c r="B52" s="8" t="s">
+      <c r="E58" s="33"/>
+    </row>
+    <row r="59" spans="2:5">
+      <c r="B59" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="C52" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D52" s="16" t="s">
+      <c r="C59" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D59" s="20" t="s">
         <v>303</v>
       </c>
-      <c r="E52" s="17"/>
-    </row>
-    <row r="53" spans="2:5">
-      <c r="B53" s="8" t="s">
+      <c r="E59" s="21"/>
+    </row>
+    <row r="60" spans="2:5">
+      <c r="B60" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="C53" s="8" t="s">
+      <c r="C60" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="D53" s="9">
+      <c r="D60" s="36">
         <v>16</v>
       </c>
-      <c r="E53" s="10"/>
-    </row>
-    <row r="54" spans="2:5">
-      <c r="B54" s="8" t="s">
+      <c r="E60" s="33"/>
+    </row>
+    <row r="61" spans="2:5">
+      <c r="B61" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="C54" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D54" s="16" t="s">
+      <c r="C61" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D61" s="20" t="s">
         <v>303</v>
       </c>
-      <c r="E54" s="17"/>
-    </row>
-    <row r="55" spans="2:5">
-      <c r="B55" s="8" t="s">
+      <c r="E61" s="21"/>
+    </row>
+    <row r="62" spans="2:5">
+      <c r="B62" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="C55" s="8" t="s">
+      <c r="C62" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="D55" s="9">
+      <c r="D62" s="36">
         <v>17</v>
       </c>
-      <c r="E55" s="10"/>
-    </row>
-    <row r="56" spans="2:5">
-      <c r="B56" s="8" t="s">
+      <c r="E62" s="33"/>
+    </row>
+    <row r="63" spans="2:5">
+      <c r="B63" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="C56" s="8" t="s">
+      <c r="C63" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="D56" s="9">
+      <c r="D63" s="36">
         <v>18</v>
       </c>
-      <c r="E56" s="10"/>
-    </row>
-    <row r="57" spans="2:5">
-      <c r="B57" s="2" t="s">
+      <c r="E63" s="33"/>
+    </row>
+    <row r="64" spans="2:5">
+      <c r="B64" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C57" s="2" t="s">
+      <c r="C64" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="D57" s="18"/>
-      <c r="E57" s="19"/>
-    </row>
-    <row r="58" spans="2:5">
-      <c r="B58" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C58" s="2" t="s">
+      <c r="D64" s="12"/>
+      <c r="E64" s="13"/>
+    </row>
+    <row r="65" spans="2:5">
+      <c r="B65" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C65" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D58" s="22"/>
-      <c r="E58" s="23"/>
-    </row>
-    <row r="59" spans="2:5">
-      <c r="B59" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C59" s="2" t="s">
+      <c r="D65" s="14"/>
+      <c r="E65" s="15"/>
+    </row>
+    <row r="66" spans="2:5">
+      <c r="B66" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C66" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D59" s="20"/>
-      <c r="E59" s="21"/>
-    </row>
-    <row r="60" spans="2:5">
-      <c r="B60" s="8" t="s">
+      <c r="D66" s="16"/>
+      <c r="E66" s="17"/>
+    </row>
+    <row r="67" spans="2:5">
+      <c r="B67" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="C60" s="8" t="s">
+      <c r="C67" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="D60" s="16" t="s">
+      <c r="D67" s="20" t="s">
         <v>303</v>
       </c>
-      <c r="E60" s="17"/>
-    </row>
-    <row r="61" spans="2:5">
-      <c r="B61" s="8" t="s">
+      <c r="E67" s="21"/>
+    </row>
+    <row r="68" spans="2:5">
+      <c r="B68" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="C61" s="8" t="s">
+      <c r="C68" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="D61" s="16" t="s">
+      <c r="D68" s="20" t="s">
         <v>303</v>
       </c>
-      <c r="E61" s="17"/>
-    </row>
-    <row r="62" spans="2:5">
-      <c r="B62" s="2" t="s">
+      <c r="E68" s="21"/>
+    </row>
+    <row r="69" spans="2:5">
+      <c r="B69" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C62" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D62" s="31"/>
-      <c r="E62" s="32"/>
-    </row>
-    <row r="63" spans="2:5">
-      <c r="B63" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="D63" s="33"/>
-      <c r="E63" s="34"/>
-    </row>
-    <row r="64" spans="2:5">
-      <c r="B64" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="C64" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="D64" s="9">
-        <v>19</v>
-      </c>
-      <c r="E64" s="10" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="65" spans="2:5">
-      <c r="B65" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="C65" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="D65" s="9">
-        <v>20</v>
-      </c>
-      <c r="E65" s="10"/>
-    </row>
-    <row r="66" spans="2:5">
-      <c r="B66" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="C66" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="D66" s="9">
-        <v>21</v>
-      </c>
-      <c r="E66" s="10"/>
-    </row>
-    <row r="67" spans="2:5">
-      <c r="B67" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="C67" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="D67" s="9">
-        <v>22</v>
-      </c>
-      <c r="E67" s="10"/>
-    </row>
-    <row r="68" spans="2:5">
-      <c r="B68" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="C68" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="D68" s="16" t="s">
-        <v>303</v>
-      </c>
-      <c r="E68" s="17"/>
-    </row>
-    <row r="69" spans="2:5">
-      <c r="B69" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="C69" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="D69" s="16" t="s">
-        <v>303</v>
-      </c>
-      <c r="E69" s="17"/>
+      <c r="C69" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D69" s="27"/>
+      <c r="E69" s="28"/>
     </row>
     <row r="70" spans="2:5">
       <c r="B70" s="2" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="D70" s="18"/>
-      <c r="E70" s="19"/>
+        <v>95</v>
+      </c>
+      <c r="D70" s="29"/>
+      <c r="E70" s="30"/>
     </row>
     <row r="71" spans="2:5">
-      <c r="B71" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="D71" s="20"/>
-      <c r="E71" s="21"/>
+      <c r="B71" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C71" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D71" s="36">
+        <v>19</v>
+      </c>
+      <c r="E71" s="33" t="s">
+        <v>305</v>
+      </c>
     </row>
     <row r="72" spans="2:5">
-      <c r="B72" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="C72" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="D72" s="16" t="s">
+      <c r="B72" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="C72" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="D72" s="36">
+        <v>20</v>
+      </c>
+      <c r="E72" s="33"/>
+    </row>
+    <row r="73" spans="2:5">
+      <c r="B73" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="C73" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="D73" s="36">
+        <v>21</v>
+      </c>
+      <c r="E73" s="33"/>
+    </row>
+    <row r="74" spans="2:5">
+      <c r="B74" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="C74" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="D74" s="36">
+        <v>22</v>
+      </c>
+      <c r="E74" s="33"/>
+    </row>
+    <row r="75" spans="2:5">
+      <c r="B75" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="C75" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="D75" s="20" t="s">
         <v>303</v>
       </c>
-      <c r="E72" s="17"/>
-    </row>
-    <row r="73" spans="2:5">
-      <c r="B73" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="C73" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D73" s="18"/>
-      <c r="E73" s="19"/>
-    </row>
-    <row r="74" spans="2:5">
-      <c r="B74" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D74" s="22"/>
-      <c r="E74" s="23"/>
-    </row>
-    <row r="75" spans="2:5">
-      <c r="B75" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="C75" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="D75" s="22"/>
-      <c r="E75" s="23"/>
+      <c r="E75" s="21"/>
     </row>
     <row r="76" spans="2:5">
-      <c r="B76" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="C76" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="D76" s="22"/>
-      <c r="E76" s="23"/>
+      <c r="B76" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C76" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="D76" s="20" t="s">
+        <v>303</v>
+      </c>
+      <c r="E76" s="21"/>
     </row>
     <row r="77" spans="2:5">
       <c r="B77" s="2" t="s">
-        <v>0</v>
+        <v>108</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="D77" s="20"/>
-      <c r="E77" s="21"/>
+        <v>109</v>
+      </c>
+      <c r="D77" s="12"/>
+      <c r="E77" s="13"/>
     </row>
     <row r="78" spans="2:5">
-      <c r="B78" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="C78" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="D78" s="9">
-        <v>23</v>
-      </c>
-      <c r="E78" s="10"/>
+      <c r="B78" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D78" s="16"/>
+      <c r="E78" s="17"/>
     </row>
     <row r="79" spans="2:5">
-      <c r="B79" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="C79" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="D79" s="9">
-        <v>24</v>
-      </c>
-      <c r="E79" s="10"/>
+      <c r="B79" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="C79" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D79" s="20" t="s">
+        <v>303</v>
+      </c>
+      <c r="E79" s="21"/>
     </row>
     <row r="80" spans="2:5">
-      <c r="B80" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="C80" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="D80" s="9">
-        <v>25</v>
-      </c>
-      <c r="E80" s="10"/>
+      <c r="B80" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D80" s="12"/>
+      <c r="E80" s="13"/>
     </row>
     <row r="81" spans="2:5">
-      <c r="B81" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="C81" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="D81" s="9">
-        <v>26</v>
-      </c>
-      <c r="E81" s="10"/>
+      <c r="B81" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D81" s="14"/>
+      <c r="E81" s="15"/>
     </row>
     <row r="82" spans="2:5">
       <c r="B82" s="2" t="s">
-        <v>0</v>
+        <v>116</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="D82" s="24"/>
-      <c r="E82" s="25"/>
+        <v>117</v>
+      </c>
+      <c r="D82" s="14"/>
+      <c r="E82" s="15"/>
     </row>
     <row r="83" spans="2:5">
-      <c r="B83" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="C83" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="D83" s="9">
-        <v>27</v>
-      </c>
-      <c r="E83" s="10"/>
+      <c r="B83" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C83" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="D83" s="14"/>
+      <c r="E83" s="15"/>
     </row>
     <row r="84" spans="2:5">
       <c r="B84" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="D84" s="18"/>
-      <c r="E84" s="26"/>
+        <v>120</v>
+      </c>
+      <c r="D84" s="16"/>
+      <c r="E84" s="17"/>
     </row>
     <row r="85" spans="2:5">
-      <c r="B85" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C85" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="D85" s="27"/>
-      <c r="E85" s="28"/>
+      <c r="B85" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="C85" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="D85" s="36">
+        <v>23</v>
+      </c>
+      <c r="E85" s="33"/>
     </row>
     <row r="86" spans="2:5">
-      <c r="B86" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C86" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="D86" s="29"/>
-      <c r="E86" s="30"/>
+      <c r="B86" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="C86" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="D86" s="36">
+        <v>24</v>
+      </c>
+      <c r="E86" s="33"/>
     </row>
     <row r="87" spans="2:5">
-      <c r="B87" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="C87" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="D87" s="9">
-        <v>28</v>
-      </c>
-      <c r="E87" s="10"/>
+      <c r="B87" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="C87" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="D87" s="36">
+        <v>25</v>
+      </c>
+      <c r="E87" s="33"/>
     </row>
     <row r="88" spans="2:5">
-      <c r="B88" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="C88" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="D88" s="9">
-        <v>29</v>
-      </c>
-      <c r="E88" s="10"/>
+      <c r="B88" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="C88" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="D88" s="36">
+        <v>26</v>
+      </c>
+      <c r="E88" s="33"/>
     </row>
     <row r="89" spans="2:5">
       <c r="B89" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="D89" s="18"/>
       <c r="E89" s="19"/>
     </row>
     <row r="90" spans="2:5">
-      <c r="B90" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="C90" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="D90" s="20"/>
-      <c r="E90" s="21"/>
+      <c r="B90" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="C90" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="D90" s="36">
+        <v>27</v>
+      </c>
+      <c r="E90" s="33"/>
     </row>
     <row r="91" spans="2:5">
-      <c r="B91" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="C91" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="D91" s="16" t="s">
-        <v>303</v>
-      </c>
-      <c r="E91" s="17"/>
+      <c r="B91" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D91" s="12"/>
+      <c r="E91" s="22"/>
     </row>
     <row r="92" spans="2:5">
       <c r="B92" s="2" t="s">
-        <v>144</v>
+        <v>0</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D92" s="18"/>
-      <c r="E92" s="19"/>
+        <v>133</v>
+      </c>
+      <c r="D92" s="23"/>
+      <c r="E92" s="24"/>
     </row>
     <row r="93" spans="2:5">
       <c r="B93" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="D93" s="22"/>
-      <c r="E93" s="23"/>
+        <v>134</v>
+      </c>
+      <c r="D93" s="25"/>
+      <c r="E93" s="26"/>
     </row>
     <row r="94" spans="2:5">
-      <c r="B94" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="C94" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="D94" s="22"/>
-      <c r="E94" s="23"/>
+      <c r="B94" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="C94" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="D94" s="36">
+        <v>28</v>
+      </c>
+      <c r="E94" s="33"/>
     </row>
     <row r="95" spans="2:5">
-      <c r="B95" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="C95" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="D95" s="22"/>
-      <c r="E95" s="23"/>
+      <c r="B95" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="C95" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="D95" s="36">
+        <v>29</v>
+      </c>
+      <c r="E95" s="33"/>
     </row>
     <row r="96" spans="2:5">
       <c r="B96" s="2" t="s">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="D96" s="22"/>
-      <c r="E96" s="23"/>
+        <v>139</v>
+      </c>
+      <c r="D96" s="12"/>
+      <c r="E96" s="13"/>
     </row>
     <row r="97" spans="2:5">
-      <c r="B97" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="C97" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="D97" s="22"/>
-      <c r="E97" s="23"/>
+      <c r="B97" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="C97" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="D97" s="16"/>
+      <c r="E97" s="17"/>
     </row>
     <row r="98" spans="2:5">
-      <c r="B98" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="C98" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="D98" s="22"/>
-      <c r="E98" s="23"/>
+      <c r="B98" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="C98" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="D98" s="20" t="s">
+        <v>303</v>
+      </c>
+      <c r="E98" s="21"/>
     </row>
     <row r="99" spans="2:5">
       <c r="B99" s="2" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="D99" s="22"/>
-      <c r="E99" s="23"/>
+        <v>0</v>
+      </c>
+      <c r="D99" s="12"/>
+      <c r="E99" s="13"/>
     </row>
     <row r="100" spans="2:5">
       <c r="B100" s="2" t="s">
-        <v>158</v>
+        <v>0</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="D100" s="22"/>
-      <c r="E100" s="23"/>
+        <v>145</v>
+      </c>
+      <c r="D100" s="14"/>
+      <c r="E100" s="15"/>
     </row>
     <row r="101" spans="2:5">
       <c r="B101" s="2" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="D101" s="22"/>
-      <c r="E101" s="23"/>
+        <v>147</v>
+      </c>
+      <c r="D101" s="14"/>
+      <c r="E101" s="15"/>
     </row>
     <row r="102" spans="2:5">
       <c r="B102" s="2" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="D102" s="22"/>
-      <c r="E102" s="23"/>
+        <v>149</v>
+      </c>
+      <c r="D102" s="14"/>
+      <c r="E102" s="15"/>
     </row>
     <row r="103" spans="2:5">
       <c r="B103" s="2" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="D103" s="22"/>
-      <c r="E103" s="23"/>
+        <v>151</v>
+      </c>
+      <c r="D103" s="14"/>
+      <c r="E103" s="15"/>
     </row>
     <row r="104" spans="2:5">
       <c r="B104" s="2" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="D104" s="22"/>
-      <c r="E104" s="23"/>
+        <v>153</v>
+      </c>
+      <c r="D104" s="14"/>
+      <c r="E104" s="15"/>
     </row>
     <row r="105" spans="2:5">
       <c r="B105" s="2" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="D105" s="22"/>
-      <c r="E105" s="23"/>
+        <v>155</v>
+      </c>
+      <c r="D105" s="14"/>
+      <c r="E105" s="15"/>
     </row>
     <row r="106" spans="2:5">
       <c r="B106" s="2" t="s">
-        <v>170</v>
+        <v>156</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="D106" s="22"/>
-      <c r="E106" s="23"/>
+        <v>157</v>
+      </c>
+      <c r="D106" s="14"/>
+      <c r="E106" s="15"/>
     </row>
     <row r="107" spans="2:5">
       <c r="B107" s="2" t="s">
-        <v>172</v>
+        <v>158</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="D107" s="22"/>
-      <c r="E107" s="23"/>
+        <v>159</v>
+      </c>
+      <c r="D107" s="14"/>
+      <c r="E107" s="15"/>
     </row>
     <row r="108" spans="2:5">
       <c r="B108" s="2" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="D108" s="22"/>
-      <c r="E108" s="23"/>
+        <v>161</v>
+      </c>
+      <c r="D108" s="14"/>
+      <c r="E108" s="15"/>
     </row>
     <row r="109" spans="2:5">
       <c r="B109" s="2" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="D109" s="22"/>
-      <c r="E109" s="23"/>
+        <v>163</v>
+      </c>
+      <c r="D109" s="14"/>
+      <c r="E109" s="15"/>
     </row>
     <row r="110" spans="2:5">
       <c r="B110" s="2" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="D110" s="22"/>
-      <c r="E110" s="23"/>
+        <v>165</v>
+      </c>
+      <c r="D110" s="14"/>
+      <c r="E110" s="15"/>
     </row>
     <row r="111" spans="2:5">
       <c r="B111" s="2" t="s">
-        <v>180</v>
+        <v>166</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D111" s="22"/>
-      <c r="E111" s="23"/>
+        <v>167</v>
+      </c>
+      <c r="D111" s="14"/>
+      <c r="E111" s="15"/>
     </row>
     <row r="112" spans="2:5">
       <c r="B112" s="2" t="s">
-        <v>181</v>
+        <v>168</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D112" s="22"/>
-      <c r="E112" s="23"/>
+        <v>169</v>
+      </c>
+      <c r="D112" s="14"/>
+      <c r="E112" s="15"/>
     </row>
     <row r="113" spans="2:5">
       <c r="B113" s="2" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="D113" s="22"/>
-      <c r="E113" s="23"/>
+        <v>171</v>
+      </c>
+      <c r="D113" s="14"/>
+      <c r="E113" s="15"/>
     </row>
     <row r="114" spans="2:5">
       <c r="B114" s="2" t="s">
-        <v>0</v>
+        <v>172</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="D114" s="22"/>
-      <c r="E114" s="23"/>
+        <v>173</v>
+      </c>
+      <c r="D114" s="14"/>
+      <c r="E114" s="15"/>
     </row>
     <row r="115" spans="2:5">
       <c r="B115" s="2" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D115" s="22"/>
-      <c r="E115" s="23"/>
+        <v>175</v>
+      </c>
+      <c r="D115" s="14"/>
+      <c r="E115" s="15"/>
     </row>
     <row r="116" spans="2:5">
       <c r="B116" s="2" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D116" s="22"/>
-      <c r="E116" s="23"/>
+        <v>177</v>
+      </c>
+      <c r="D116" s="14"/>
+      <c r="E116" s="15"/>
     </row>
     <row r="117" spans="2:5">
       <c r="B117" s="2" t="s">
-        <v>0</v>
+        <v>178</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="D117" s="22"/>
-      <c r="E117" s="23"/>
+        <v>179</v>
+      </c>
+      <c r="D117" s="14"/>
+      <c r="E117" s="15"/>
     </row>
     <row r="118" spans="2:5">
       <c r="B118" s="2" t="s">
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="D118" s="22"/>
-      <c r="E118" s="23"/>
+        <v>0</v>
+      </c>
+      <c r="D118" s="14"/>
+      <c r="E118" s="15"/>
     </row>
     <row r="119" spans="2:5">
       <c r="B119" s="2" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="C119" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D119" s="22"/>
-      <c r="E119" s="23"/>
+      <c r="D119" s="14"/>
+      <c r="E119" s="15"/>
     </row>
     <row r="120" spans="2:5">
       <c r="B120" s="2" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="D120" s="22"/>
-      <c r="E120" s="23"/>
+        <v>183</v>
+      </c>
+      <c r="D120" s="14"/>
+      <c r="E120" s="15"/>
     </row>
     <row r="121" spans="2:5">
       <c r="B121" s="2" t="s">
-        <v>192</v>
+        <v>0</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="D121" s="22"/>
-      <c r="E121" s="23"/>
+        <v>184</v>
+      </c>
+      <c r="D121" s="14"/>
+      <c r="E121" s="15"/>
     </row>
     <row r="122" spans="2:5">
       <c r="B122" s="2" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="D122" s="22"/>
-      <c r="E122" s="23"/>
+        <v>0</v>
+      </c>
+      <c r="D122" s="14"/>
+      <c r="E122" s="15"/>
     </row>
     <row r="123" spans="2:5">
       <c r="B123" s="2" t="s">
-        <v>0</v>
+        <v>186</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="D123" s="20"/>
-      <c r="E123" s="21"/>
+        <v>0</v>
+      </c>
+      <c r="D123" s="14"/>
+      <c r="E123" s="15"/>
     </row>
     <row r="124" spans="2:5">
-      <c r="B124" s="8" t="s">
-        <v>197</v>
-      </c>
-      <c r="C124" s="8" t="s">
-        <v>198</v>
-      </c>
-      <c r="D124" s="15">
-        <v>30</v>
-      </c>
-      <c r="E124" s="10"/>
+      <c r="B124" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C124" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="D124" s="14"/>
+      <c r="E124" s="15"/>
     </row>
     <row r="125" spans="2:5">
       <c r="B125" s="2" t="s">
-        <v>199</v>
+        <v>0</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="D125" s="24"/>
-      <c r="E125" s="25"/>
+        <v>188</v>
+      </c>
+      <c r="D125" s="14"/>
+      <c r="E125" s="15"/>
     </row>
     <row r="126" spans="2:5">
-      <c r="B126" s="8" t="s">
-        <v>201</v>
-      </c>
-      <c r="C126" s="8" t="s">
-        <v>202</v>
-      </c>
-      <c r="D126" s="9">
-        <v>31</v>
-      </c>
-      <c r="E126" s="10"/>
+      <c r="B126" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C126" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D126" s="14"/>
+      <c r="E126" s="15"/>
     </row>
     <row r="127" spans="2:5">
       <c r="B127" s="2" t="s">
-        <v>0</v>
+        <v>190</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="D127" s="18"/>
-      <c r="E127" s="19"/>
+        <v>191</v>
+      </c>
+      <c r="D127" s="14"/>
+      <c r="E127" s="15"/>
     </row>
     <row r="128" spans="2:5">
       <c r="B128" s="2" t="s">
-        <v>0</v>
+        <v>192</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="D128" s="20"/>
-      <c r="E128" s="21"/>
+        <v>193</v>
+      </c>
+      <c r="D128" s="14"/>
+      <c r="E128" s="15"/>
     </row>
     <row r="129" spans="2:5">
-      <c r="B129" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="C129" s="8" t="s">
-        <v>205</v>
-      </c>
-      <c r="D129" s="14">
-        <v>32</v>
-      </c>
-      <c r="E129" s="14" t="s">
-        <v>300</v>
-      </c>
+      <c r="B129" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="C129" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="D129" s="14"/>
+      <c r="E129" s="15"/>
     </row>
     <row r="130" spans="2:5">
       <c r="B130" s="2" t="s">
-        <v>206</v>
+        <v>0</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D130" s="18"/>
-      <c r="E130" s="19"/>
+        <v>196</v>
+      </c>
+      <c r="D130" s="16"/>
+      <c r="E130" s="17"/>
     </row>
     <row r="131" spans="2:5">
-      <c r="B131" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C131" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="D131" s="22"/>
-      <c r="E131" s="23"/>
+      <c r="B131" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="C131" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="D131" s="37">
+        <v>30</v>
+      </c>
+      <c r="E131" s="33"/>
     </row>
     <row r="132" spans="2:5">
       <c r="B132" s="2" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="D132" s="22"/>
-      <c r="E132" s="23"/>
+        <v>200</v>
+      </c>
+      <c r="D132" s="18"/>
+      <c r="E132" s="19"/>
     </row>
     <row r="133" spans="2:5">
-      <c r="B133" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C133" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="D133" s="22"/>
-      <c r="E133" s="23"/>
+      <c r="B133" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="C133" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="D133" s="36">
+        <v>31</v>
+      </c>
+      <c r="E133" s="33"/>
     </row>
     <row r="134" spans="2:5">
       <c r="B134" s="2" t="s">
-        <v>211</v>
+        <v>0</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D134" s="22"/>
-      <c r="E134" s="23"/>
+        <v>203</v>
+      </c>
+      <c r="D134" s="12"/>
+      <c r="E134" s="13"/>
     </row>
     <row r="135" spans="2:5">
       <c r="B135" s="2" t="s">
-        <v>212</v>
+        <v>0</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="D135" s="22"/>
-      <c r="E135" s="23"/>
+        <v>204</v>
+      </c>
+      <c r="D135" s="16"/>
+      <c r="E135" s="17"/>
     </row>
     <row r="136" spans="2:5">
-      <c r="B136" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C136" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="D136" s="22"/>
-      <c r="E136" s="23"/>
+      <c r="B136" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C136" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="D136" s="36">
+        <v>32</v>
+      </c>
+      <c r="E136" s="34" t="s">
+        <v>300</v>
+      </c>
     </row>
     <row r="137" spans="2:5">
       <c r="B137" s="2" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="D137" s="22"/>
-      <c r="E137" s="23"/>
+        <v>0</v>
+      </c>
+      <c r="D137" s="12"/>
+      <c r="E137" s="13"/>
     </row>
     <row r="138" spans="2:5">
       <c r="B138" s="2" t="s">
-        <v>217</v>
+        <v>0</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="D138" s="22"/>
-      <c r="E138" s="23"/>
+        <v>207</v>
+      </c>
+      <c r="D138" s="14"/>
+      <c r="E138" s="15"/>
     </row>
     <row r="139" spans="2:5">
       <c r="B139" s="2" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="D139" s="22"/>
-      <c r="E139" s="23"/>
+        <v>209</v>
+      </c>
+      <c r="D139" s="14"/>
+      <c r="E139" s="15"/>
     </row>
     <row r="140" spans="2:5">
       <c r="B140" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="D140" s="22"/>
-      <c r="E140" s="23"/>
+        <v>210</v>
+      </c>
+      <c r="D140" s="14"/>
+      <c r="E140" s="15"/>
     </row>
     <row r="141" spans="2:5">
       <c r="B141" s="2" t="s">
-        <v>0</v>
+        <v>211</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="D141" s="22"/>
-      <c r="E141" s="23"/>
+        <v>0</v>
+      </c>
+      <c r="D141" s="14"/>
+      <c r="E141" s="15"/>
     </row>
     <row r="142" spans="2:5">
       <c r="B142" s="2" t="s">
-        <v>0</v>
+        <v>212</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="D142" s="22"/>
-      <c r="E142" s="23"/>
+        <v>213</v>
+      </c>
+      <c r="D142" s="14"/>
+      <c r="E142" s="15"/>
     </row>
     <row r="143" spans="2:5">
       <c r="B143" s="2" t="s">
-        <v>224</v>
+        <v>0</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="D143" s="22"/>
-      <c r="E143" s="23"/>
+        <v>214</v>
+      </c>
+      <c r="D143" s="14"/>
+      <c r="E143" s="15"/>
     </row>
     <row r="144" spans="2:5">
       <c r="B144" s="2" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D144" s="22"/>
-      <c r="E144" s="23"/>
+        <v>216</v>
+      </c>
+      <c r="D144" s="14"/>
+      <c r="E144" s="15"/>
     </row>
     <row r="145" spans="2:5">
       <c r="B145" s="2" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="D145" s="22"/>
-      <c r="E145" s="23"/>
+        <v>218</v>
+      </c>
+      <c r="D145" s="14"/>
+      <c r="E145" s="15"/>
     </row>
     <row r="146" spans="2:5">
       <c r="B146" s="2" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="D146" s="22"/>
-      <c r="E146" s="23"/>
+        <v>220</v>
+      </c>
+      <c r="D146" s="14"/>
+      <c r="E146" s="15"/>
     </row>
     <row r="147" spans="2:5">
       <c r="B147" s="2" t="s">
-        <v>231</v>
+        <v>0</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="D147" s="22"/>
-      <c r="E147" s="23"/>
+        <v>221</v>
+      </c>
+      <c r="D147" s="14"/>
+      <c r="E147" s="15"/>
     </row>
     <row r="148" spans="2:5">
       <c r="B148" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="D148" s="22"/>
-      <c r="E148" s="23"/>
+        <v>222</v>
+      </c>
+      <c r="D148" s="14"/>
+      <c r="E148" s="15"/>
     </row>
     <row r="149" spans="2:5">
       <c r="B149" s="2" t="s">
-        <v>234</v>
+        <v>0</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="D149" s="22"/>
-      <c r="E149" s="23"/>
+        <v>223</v>
+      </c>
+      <c r="D149" s="14"/>
+      <c r="E149" s="15"/>
     </row>
     <row r="150" spans="2:5">
       <c r="B150" s="2" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="D150" s="22"/>
-      <c r="E150" s="23"/>
+        <v>225</v>
+      </c>
+      <c r="D150" s="14"/>
+      <c r="E150" s="15"/>
     </row>
     <row r="151" spans="2:5">
       <c r="B151" s="2" t="s">
-        <v>238</v>
+        <v>226</v>
       </c>
       <c r="C151" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D151" s="20"/>
-      <c r="E151" s="21"/>
+      <c r="D151" s="14"/>
+      <c r="E151" s="15"/>
     </row>
     <row r="152" spans="2:5">
-      <c r="B152" s="8" t="s">
-        <v>239</v>
-      </c>
-      <c r="C152" s="8" t="s">
-        <v>240</v>
-      </c>
-      <c r="D152" s="16" t="s">
-        <v>303</v>
-      </c>
-      <c r="E152" s="17"/>
+      <c r="B152" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="C152" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D152" s="14"/>
+      <c r="E152" s="15"/>
     </row>
     <row r="153" spans="2:5">
       <c r="B153" s="2" t="s">
-        <v>241</v>
+        <v>229</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="D153" s="18"/>
-      <c r="E153" s="19"/>
+        <v>230</v>
+      </c>
+      <c r="D153" s="14"/>
+      <c r="E153" s="15"/>
     </row>
     <row r="154" spans="2:5">
       <c r="B154" s="2" t="s">
-        <v>243</v>
+        <v>231</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="D154" s="22"/>
-      <c r="E154" s="23"/>
+        <v>232</v>
+      </c>
+      <c r="D154" s="14"/>
+      <c r="E154" s="15"/>
     </row>
     <row r="155" spans="2:5">
       <c r="B155" s="2" t="s">
-        <v>245</v>
+        <v>0</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="D155" s="22"/>
-      <c r="E155" s="23"/>
+        <v>233</v>
+      </c>
+      <c r="D155" s="14"/>
+      <c r="E155" s="15"/>
     </row>
     <row r="156" spans="2:5">
       <c r="B156" s="2" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="D156" s="22"/>
-      <c r="E156" s="23"/>
+        <v>235</v>
+      </c>
+      <c r="D156" s="14"/>
+      <c r="E156" s="15"/>
     </row>
     <row r="157" spans="2:5">
       <c r="B157" s="2" t="s">
-        <v>249</v>
+        <v>236</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="D157" s="22"/>
-      <c r="E157" s="23"/>
+        <v>237</v>
+      </c>
+      <c r="D157" s="14"/>
+      <c r="E157" s="15"/>
     </row>
     <row r="158" spans="2:5">
       <c r="B158" s="2" t="s">
-        <v>251</v>
+        <v>238</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="D158" s="22"/>
-      <c r="E158" s="23"/>
+        <v>0</v>
+      </c>
+      <c r="D158" s="16"/>
+      <c r="E158" s="17"/>
     </row>
     <row r="159" spans="2:5">
-      <c r="B159" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="C159" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="D159" s="22"/>
-      <c r="E159" s="23"/>
+      <c r="B159" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="C159" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="D159" s="20" t="s">
+        <v>303</v>
+      </c>
+      <c r="E159" s="21"/>
     </row>
     <row r="160" spans="2:5">
       <c r="B160" s="2" t="s">
-        <v>255</v>
+        <v>241</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="D160" s="22"/>
-      <c r="E160" s="23"/>
+        <v>242</v>
+      </c>
+      <c r="D160" s="12"/>
+      <c r="E160" s="13"/>
     </row>
     <row r="161" spans="2:5">
       <c r="B161" s="2" t="s">
-        <v>257</v>
+        <v>243</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D161" s="20"/>
-      <c r="E161" s="21"/>
+        <v>244</v>
+      </c>
+      <c r="D161" s="14"/>
+      <c r="E161" s="15"/>
     </row>
     <row r="162" spans="2:5">
-      <c r="B162" s="8" t="s">
-        <v>258</v>
-      </c>
-      <c r="C162" s="8" t="s">
-        <v>259</v>
-      </c>
-      <c r="D162" s="9">
-        <v>33</v>
-      </c>
-      <c r="E162" s="10"/>
+      <c r="B162" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="C162" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="D162" s="14"/>
+      <c r="E162" s="15"/>
     </row>
     <row r="163" spans="2:5">
-      <c r="B163" s="8" t="s">
-        <v>260</v>
-      </c>
-      <c r="C163" s="8" t="s">
-        <v>261</v>
-      </c>
-      <c r="D163" s="16" t="s">
-        <v>303</v>
-      </c>
-      <c r="E163" s="17"/>
+      <c r="B163" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="C163" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="D163" s="14"/>
+      <c r="E163" s="15"/>
     </row>
     <row r="164" spans="2:5">
-      <c r="B164" s="8" t="s">
-        <v>262</v>
-      </c>
-      <c r="C164" s="8" t="s">
-        <v>263</v>
-      </c>
-      <c r="D164" s="9">
-        <v>34</v>
-      </c>
-      <c r="E164" s="10"/>
+      <c r="B164" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="C164" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="D164" s="14"/>
+      <c r="E164" s="15"/>
     </row>
     <row r="165" spans="2:5">
       <c r="B165" s="2" t="s">
-        <v>264</v>
+        <v>251</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="D165" s="18"/>
-      <c r="E165" s="19"/>
+        <v>252</v>
+      </c>
+      <c r="D165" s="14"/>
+      <c r="E165" s="15"/>
     </row>
     <row r="166" spans="2:5">
       <c r="B166" s="2" t="s">
-        <v>266</v>
+        <v>253</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>267</v>
-      </c>
-      <c r="D166" s="22"/>
-      <c r="E166" s="23"/>
+        <v>254</v>
+      </c>
+      <c r="D166" s="14"/>
+      <c r="E166" s="15"/>
     </row>
     <row r="167" spans="2:5">
       <c r="B167" s="2" t="s">
-        <v>268</v>
+        <v>255</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>269</v>
-      </c>
-      <c r="D167" s="22"/>
-      <c r="E167" s="23"/>
+        <v>256</v>
+      </c>
+      <c r="D167" s="14"/>
+      <c r="E167" s="15"/>
     </row>
     <row r="168" spans="2:5">
       <c r="B168" s="2" t="s">
-        <v>270</v>
+        <v>257</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>271</v>
-      </c>
-      <c r="D168" s="22"/>
-      <c r="E168" s="23"/>
+        <v>0</v>
+      </c>
+      <c r="D168" s="16"/>
+      <c r="E168" s="17"/>
     </row>
     <row r="169" spans="2:5">
-      <c r="B169" s="2" t="s">
-        <v>272</v>
-      </c>
-      <c r="C169" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="D169" s="22"/>
-      <c r="E169" s="23"/>
+      <c r="B169" s="7" t="s">
+        <v>258</v>
+      </c>
+      <c r="C169" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="D169" s="36">
+        <v>33</v>
+      </c>
+      <c r="E169" s="33"/>
     </row>
     <row r="170" spans="2:5">
-      <c r="B170" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="C170" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="D170" s="22"/>
-      <c r="E170" s="23"/>
+      <c r="B170" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="C170" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="D170" s="20" t="s">
+        <v>303</v>
+      </c>
+      <c r="E170" s="21"/>
     </row>
     <row r="171" spans="2:5">
-      <c r="B171" s="2" t="s">
-        <v>276</v>
-      </c>
-      <c r="C171" s="2" t="s">
-        <v>277</v>
-      </c>
-      <c r="D171" s="22"/>
-      <c r="E171" s="23"/>
+      <c r="B171" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="C171" s="7" t="s">
+        <v>263</v>
+      </c>
+      <c r="D171" s="36">
+        <v>34</v>
+      </c>
+      <c r="E171" s="33"/>
     </row>
     <row r="172" spans="2:5">
       <c r="B172" s="2" t="s">
-        <v>278</v>
+        <v>264</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="D172" s="22"/>
-      <c r="E172" s="23"/>
+        <v>265</v>
+      </c>
+      <c r="D172" s="12"/>
+      <c r="E172" s="13"/>
     </row>
     <row r="173" spans="2:5">
       <c r="B173" s="2" t="s">
-        <v>280</v>
+        <v>266</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D173" s="22"/>
-      <c r="E173" s="23"/>
+        <v>267</v>
+      </c>
+      <c r="D173" s="14"/>
+      <c r="E173" s="15"/>
     </row>
     <row r="174" spans="2:5">
       <c r="B174" s="2" t="s">
-        <v>281</v>
+        <v>268</v>
       </c>
       <c r="C174" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="D174" s="22"/>
-      <c r="E174" s="23"/>
+        <v>269</v>
+      </c>
+      <c r="D174" s="14"/>
+      <c r="E174" s="15"/>
     </row>
     <row r="175" spans="2:5">
       <c r="B175" s="2" t="s">
-        <v>0</v>
+        <v>270</v>
       </c>
       <c r="C175" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="D175" s="22"/>
-      <c r="E175" s="23"/>
+        <v>271</v>
+      </c>
+      <c r="D175" s="14"/>
+      <c r="E175" s="15"/>
     </row>
     <row r="176" spans="2:5">
       <c r="B176" s="2" t="s">
-        <v>0</v>
+        <v>272</v>
       </c>
       <c r="C176" s="2" t="s">
-        <v>284</v>
-      </c>
-      <c r="D176" s="22"/>
-      <c r="E176" s="23"/>
+        <v>273</v>
+      </c>
+      <c r="D176" s="14"/>
+      <c r="E176" s="15"/>
     </row>
     <row r="177" spans="2:5">
       <c r="B177" s="2" t="s">
-        <v>0</v>
+        <v>274</v>
       </c>
       <c r="C177" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="D177" s="22"/>
-      <c r="E177" s="23"/>
+        <v>275</v>
+      </c>
+      <c r="D177" s="14"/>
+      <c r="E177" s="15"/>
     </row>
     <row r="178" spans="2:5">
       <c r="B178" s="2" t="s">
-        <v>0</v>
+        <v>276</v>
       </c>
       <c r="C178" s="2" t="s">
-        <v>286</v>
-      </c>
-      <c r="D178" s="22"/>
-      <c r="E178" s="23"/>
+        <v>277</v>
+      </c>
+      <c r="D178" s="14"/>
+      <c r="E178" s="15"/>
     </row>
     <row r="179" spans="2:5">
       <c r="B179" s="2" t="s">
-        <v>287</v>
+        <v>278</v>
       </c>
       <c r="C179" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D179" s="22"/>
-      <c r="E179" s="23"/>
+        <v>279</v>
+      </c>
+      <c r="D179" s="14"/>
+      <c r="E179" s="15"/>
     </row>
     <row r="180" spans="2:5">
       <c r="B180" s="2" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="C180" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D180" s="22"/>
-      <c r="E180" s="23"/>
+      <c r="D180" s="14"/>
+      <c r="E180" s="15"/>
     </row>
     <row r="181" spans="2:5">
       <c r="B181" s="2" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="C181" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D181" s="22"/>
-      <c r="E181" s="23"/>
+        <v>282</v>
+      </c>
+      <c r="D181" s="14"/>
+      <c r="E181" s="15"/>
     </row>
     <row r="182" spans="2:5">
       <c r="B182" s="2" t="s">
-        <v>290</v>
+        <v>0</v>
       </c>
       <c r="C182" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D182" s="22"/>
-      <c r="E182" s="23"/>
+        <v>283</v>
+      </c>
+      <c r="D182" s="14"/>
+      <c r="E182" s="15"/>
     </row>
     <row r="183" spans="2:5">
       <c r="B183" s="2" t="s">
-        <v>291</v>
+        <v>0</v>
       </c>
       <c r="C183" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D183" s="20"/>
-      <c r="E183" s="21"/>
+        <v>284</v>
+      </c>
+      <c r="D183" s="14"/>
+      <c r="E183" s="15"/>
     </row>
     <row r="184" spans="2:5">
-      <c r="B184" s="8" t="s">
-        <v>292</v>
-      </c>
-      <c r="C184" s="8" t="s">
-        <v>293</v>
-      </c>
-      <c r="D184" s="9">
-        <v>35</v>
-      </c>
-      <c r="E184" s="10"/>
+      <c r="B184" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C184" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="D184" s="14"/>
+      <c r="E184" s="15"/>
     </row>
     <row r="185" spans="2:5">
       <c r="B185" s="2" t="s">
-        <v>294</v>
+        <v>0</v>
       </c>
       <c r="C185" s="2" t="s">
-        <v>295</v>
-      </c>
-      <c r="D185" s="18"/>
-      <c r="E185" s="19"/>
+        <v>286</v>
+      </c>
+      <c r="D185" s="14"/>
+      <c r="E185" s="15"/>
     </row>
     <row r="186" spans="2:5">
       <c r="B186" s="2" t="s">
-        <v>0</v>
+        <v>287</v>
       </c>
       <c r="C186" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D186" s="14"/>
+      <c r="E186" s="15"/>
+    </row>
+    <row r="187" spans="2:5">
+      <c r="B187" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="C187" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D187" s="14"/>
+      <c r="E187" s="15"/>
+    </row>
+    <row r="188" spans="2:5">
+      <c r="B188" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="C188" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D188" s="14"/>
+      <c r="E188" s="15"/>
+    </row>
+    <row r="189" spans="2:5">
+      <c r="B189" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="C189" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D189" s="14"/>
+      <c r="E189" s="15"/>
+    </row>
+    <row r="190" spans="2:5">
+      <c r="B190" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="C190" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D190" s="16"/>
+      <c r="E190" s="17"/>
+    </row>
+    <row r="191" spans="2:5">
+      <c r="B191" s="7" t="s">
+        <v>292</v>
+      </c>
+      <c r="C191" s="7" t="s">
+        <v>293</v>
+      </c>
+      <c r="D191" s="36">
+        <v>35</v>
+      </c>
+      <c r="E191" s="33"/>
+    </row>
+    <row r="192" spans="2:5">
+      <c r="B192" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="C192" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="D192" s="12"/>
+      <c r="E192" s="13"/>
+    </row>
+    <row r="193" spans="2:5">
+      <c r="B193" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C193" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="D186" s="20"/>
-      <c r="E186" s="21"/>
+      <c r="D193" s="16"/>
+      <c r="E193" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="41">
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D8:E19"/>
-    <mergeCell ref="D21:E22"/>
-    <mergeCell ref="D27:E30"/>
+  <mergeCells count="49">
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="D76:E76"/>
+    <mergeCell ref="D98:E98"/>
+    <mergeCell ref="D159:E159"/>
+    <mergeCell ref="D170:E170"/>
+    <mergeCell ref="D77:E78"/>
+    <mergeCell ref="D134:E135"/>
+    <mergeCell ref="D137:E158"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="D67:E67"/>
+    <mergeCell ref="D68:E68"/>
+    <mergeCell ref="D75:E75"/>
+    <mergeCell ref="D192:E193"/>
+    <mergeCell ref="D80:E84"/>
+    <mergeCell ref="D96:E97"/>
+    <mergeCell ref="D99:E130"/>
+    <mergeCell ref="D132:E132"/>
+    <mergeCell ref="D160:E168"/>
+    <mergeCell ref="D172:E190"/>
+    <mergeCell ref="D89:E89"/>
+    <mergeCell ref="D91:E93"/>
+    <mergeCell ref="D64:E66"/>
+    <mergeCell ref="D69:E70"/>
+    <mergeCell ref="D79:E79"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D15:E26"/>
+    <mergeCell ref="D28:E29"/>
+    <mergeCell ref="D34:E37"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D40:E40"/>
     <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="D68:E68"/>
-    <mergeCell ref="D185:E186"/>
-    <mergeCell ref="D73:E77"/>
-    <mergeCell ref="D89:E90"/>
-    <mergeCell ref="D92:E123"/>
-    <mergeCell ref="D125:E125"/>
-    <mergeCell ref="D153:E161"/>
-    <mergeCell ref="D165:E183"/>
-    <mergeCell ref="D82:E82"/>
-    <mergeCell ref="D84:E86"/>
-    <mergeCell ref="D57:E59"/>
-    <mergeCell ref="D62:E63"/>
     <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D72:E72"/>
-    <mergeCell ref="D69:E69"/>
-    <mergeCell ref="D91:E91"/>
-    <mergeCell ref="D152:E152"/>
-    <mergeCell ref="D163:E163"/>
-    <mergeCell ref="D70:E71"/>
-    <mergeCell ref="D127:E128"/>
-    <mergeCell ref="D130:E151"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>